<commit_message>
Update: modificação do arquivo Documentação.docx
</commit_message>
<xml_diff>
--- a/Documentacao/Backlog.xlsx
+++ b/Documentacao/Backlog.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Harison\Downloads\Umitrix\Documentacao\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://bandteccom-my.sharepoint.com/personal/erick_hlee_sptech_school/Documents/SPTECH/.Sprint 2/UMITRIX/Documentacao/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{A018D417-40FE-474A-8F9C-A9145FFFA906}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="13" documentId="8_{A018D417-40FE-474A-8F9C-A9145FFFA906}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B09435AC-DE4D-4A50-BAF4-AA435D7375AC}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView minimized="1" xWindow="2340" yWindow="2340" windowWidth="18000" windowHeight="9810" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="69">
   <si>
     <t>Projeto Umi - Backlog</t>
   </si>
@@ -200,9 +200,6 @@
     <t>Esquema Inicial do Banco de Dados</t>
   </si>
   <si>
-    <t>Plano que define como os dados serão organizados e relacionados.</t>
-  </si>
-  <si>
     <t>Organização Trello</t>
   </si>
   <si>
@@ -236,17 +233,23 @@
     <t>Avaliação e ajustes</t>
   </si>
   <si>
-    <t>Garantia de desempenho e funcionalidade pelo Feed Back e a análise da aplicação.</t>
-  </si>
-  <si>
     <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t>Colcoar id</t>
+  </si>
+  <si>
+    <t>Plano que define como os que dados serão organizados e relacionados.</t>
+  </si>
+  <si>
+    <t>Garantia de desempenho e funcionalidade pelo Feedback e a análise da aplicação.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="10" x14ac:knownFonts="1">
+  <fonts count="14" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -307,8 +310,35 @@
       <sz val="12"/>
       <name val="Verdana"/>
     </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color rgb="FFFF0000"/>
+      <name val="Verdana"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="9"/>
+      <name val="Verdana"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color rgb="FFC00000"/>
+      <name val="Verdana"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <name val="Verdana"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -324,6 +354,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.249977111117893"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -381,7 +417,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -428,6 +464,48 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -763,35 +841,38 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="F2:M53"/>
+  <dimension ref="E2:M53"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="G7" sqref="G7"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="G34" sqref="G34"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="4" max="4" width="12.5546875" customWidth="1"/>
-    <col min="5" max="5" width="12.6640625" customWidth="1"/>
+    <col min="4" max="4" width="12.5" customWidth="1"/>
+    <col min="5" max="5" width="12.625" customWidth="1"/>
     <col min="6" max="6" width="54" customWidth="1"/>
-    <col min="7" max="7" width="153.33203125" customWidth="1"/>
-    <col min="8" max="8" width="24.33203125" style="4" customWidth="1"/>
-    <col min="13" max="13" width="36.33203125" customWidth="1"/>
+    <col min="7" max="7" width="153.375" customWidth="1"/>
+    <col min="8" max="8" width="24.375" style="4" customWidth="1"/>
+    <col min="13" max="13" width="36.375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="6:13" ht="67.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="5:13" ht="67.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="F2" s="16" t="s">
         <v>0</v>
       </c>
       <c r="G2" s="16"/>
       <c r="H2" s="16"/>
     </row>
-    <row r="3" spans="6:13" s="11" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="5:13" s="11" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="F3" s="12"/>
       <c r="G3" s="12"/>
       <c r="H3" s="12"/>
     </row>
-    <row r="4" spans="6:13" s="4" customFormat="1" ht="36" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="5:13" s="4" customFormat="1" ht="36" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="E4" s="4" t="s">
+        <v>66</v>
+      </c>
       <c r="F4" s="13" t="s">
         <v>1</v>
       </c>
@@ -802,7 +883,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="6:13" s="2" customFormat="1" ht="39.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="5:13" s="2" customFormat="1" ht="39.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="F5" s="5" t="s">
         <v>4</v>
       </c>
@@ -814,19 +895,19 @@
       </c>
       <c r="M5" s="3"/>
     </row>
-    <row r="6" spans="6:13" s="2" customFormat="1" ht="39.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="F6" s="5" t="s">
+    <row r="6" spans="5:13" s="2" customFormat="1" ht="39.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="F6" s="17" t="s">
         <v>7</v>
       </c>
-      <c r="G6" s="6" t="s">
+      <c r="G6" s="18" t="s">
         <v>8</v>
       </c>
-      <c r="H6" s="7" t="s">
+      <c r="H6" s="19" t="s">
         <v>6</v>
       </c>
       <c r="M6" s="3"/>
     </row>
-    <row r="7" spans="6:13" s="2" customFormat="1" ht="39.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="5:13" s="2" customFormat="1" ht="39.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="F7" s="5" t="s">
         <v>9</v>
       </c>
@@ -838,7 +919,7 @@
       </c>
       <c r="M7" s="3"/>
     </row>
-    <row r="8" spans="6:13" s="2" customFormat="1" ht="39.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="5:13" s="2" customFormat="1" ht="39.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="F8" s="5" t="s">
         <v>11</v>
       </c>
@@ -850,7 +931,7 @@
       </c>
       <c r="M8" s="3"/>
     </row>
-    <row r="9" spans="6:13" s="2" customFormat="1" ht="39.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="5:13" s="2" customFormat="1" ht="39.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="F9" s="5" t="s">
         <v>13</v>
       </c>
@@ -862,7 +943,7 @@
       </c>
       <c r="M9" s="3"/>
     </row>
-    <row r="10" spans="6:13" s="2" customFormat="1" ht="39.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="5:13" s="2" customFormat="1" ht="39.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="F10" s="5" t="s">
         <v>15</v>
       </c>
@@ -874,7 +955,7 @@
       </c>
       <c r="M10" s="3"/>
     </row>
-    <row r="11" spans="6:13" s="2" customFormat="1" ht="39.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="5:13" s="2" customFormat="1" ht="39.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="F11" s="5" t="s">
         <v>17</v>
       </c>
@@ -886,7 +967,7 @@
       </c>
       <c r="M11" s="3"/>
     </row>
-    <row r="12" spans="6:13" s="2" customFormat="1" ht="39.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="5:13" s="2" customFormat="1" ht="39.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="F12" s="5" t="s">
         <v>19</v>
       </c>
@@ -898,7 +979,7 @@
       </c>
       <c r="M12" s="3"/>
     </row>
-    <row r="13" spans="6:13" s="2" customFormat="1" ht="39.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="5:13" s="2" customFormat="1" ht="39.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="F13" s="5" t="s">
         <v>21</v>
       </c>
@@ -910,7 +991,7 @@
       </c>
       <c r="M13" s="3"/>
     </row>
-    <row r="14" spans="6:13" s="2" customFormat="1" ht="39.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="5:13" s="2" customFormat="1" ht="39.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="F14" s="5" t="s">
         <v>23</v>
       </c>
@@ -922,7 +1003,7 @@
       </c>
       <c r="M14" s="3"/>
     </row>
-    <row r="15" spans="6:13" s="2" customFormat="1" ht="39.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="5:13" s="2" customFormat="1" ht="39.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="F15" s="5" t="s">
         <v>25</v>
       </c>
@@ -934,7 +1015,7 @@
       </c>
       <c r="M15" s="3"/>
     </row>
-    <row r="16" spans="6:13" s="2" customFormat="1" ht="39.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="5:13" s="2" customFormat="1" ht="39.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="F16" s="5" t="s">
         <v>27</v>
       </c>
@@ -946,7 +1027,7 @@
       </c>
       <c r="M16" s="3"/>
     </row>
-    <row r="17" spans="6:13" s="2" customFormat="1" ht="39.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="6:13" s="2" customFormat="1" ht="39.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="F17" s="5" t="s">
         <v>29</v>
       </c>
@@ -958,19 +1039,19 @@
       </c>
       <c r="M17" s="3"/>
     </row>
-    <row r="18" spans="6:13" s="2" customFormat="1" ht="39.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="F18" s="5" t="s">
+    <row r="18" spans="6:13" s="2" customFormat="1" ht="39.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="F18" s="20" t="s">
         <v>31</v>
       </c>
-      <c r="G18" s="6" t="s">
+      <c r="G18" s="21" t="s">
         <v>32</v>
       </c>
-      <c r="H18" s="7" t="s">
+      <c r="H18" s="22" t="s">
         <v>6</v>
       </c>
       <c r="M18" s="3"/>
     </row>
-    <row r="19" spans="6:13" s="2" customFormat="1" ht="39.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="6:13" s="2" customFormat="1" ht="39.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="F19" s="5" t="s">
         <v>33</v>
       </c>
@@ -982,7 +1063,7 @@
       </c>
       <c r="M19" s="3"/>
     </row>
-    <row r="20" spans="6:13" s="2" customFormat="1" ht="39.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="6:13" s="2" customFormat="1" ht="39.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="F20" s="5" t="s">
         <v>36</v>
       </c>
@@ -994,7 +1075,7 @@
       </c>
       <c r="M20" s="3"/>
     </row>
-    <row r="21" spans="6:13" s="2" customFormat="1" ht="39.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="6:13" s="2" customFormat="1" ht="39.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="F21" s="5" t="s">
         <v>38</v>
       </c>
@@ -1006,7 +1087,7 @@
       </c>
       <c r="M21" s="3"/>
     </row>
-    <row r="22" spans="6:13" s="2" customFormat="1" ht="39.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="6:13" s="2" customFormat="1" ht="39.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="F22" s="5" t="s">
         <v>40</v>
       </c>
@@ -1018,7 +1099,7 @@
       </c>
       <c r="M22" s="3"/>
     </row>
-    <row r="23" spans="6:13" s="2" customFormat="1" ht="39.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="6:13" s="2" customFormat="1" ht="39.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="F23" s="5" t="s">
         <v>42</v>
       </c>
@@ -1030,7 +1111,7 @@
       </c>
       <c r="M23" s="3"/>
     </row>
-    <row r="24" spans="6:13" s="2" customFormat="1" ht="39.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="6:13" s="2" customFormat="1" ht="39.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="F24" s="5" t="s">
         <v>44</v>
       </c>
@@ -1041,215 +1122,216 @@
         <v>46</v>
       </c>
     </row>
-    <row r="25" spans="6:13" s="2" customFormat="1" ht="39.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="F25" s="5" t="s">
+    <row r="25" spans="6:13" s="2" customFormat="1" ht="39.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="F25" s="23" t="s">
         <v>47</v>
       </c>
-      <c r="G25" s="6" t="s">
+      <c r="G25" s="24" t="s">
         <v>48</v>
       </c>
-      <c r="H25" s="9" t="s">
+      <c r="H25" s="25" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="26" spans="6:13" s="2" customFormat="1" ht="39.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="F26" s="5" t="s">
+    <row r="26" spans="6:13" s="2" customFormat="1" ht="39.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="F26" s="26" t="s">
         <v>49</v>
       </c>
-      <c r="G26" s="6" t="s">
+      <c r="G26" s="27" t="s">
         <v>50</v>
       </c>
       <c r="H26" s="9" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="27" spans="6:13" s="2" customFormat="1" ht="39.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="F27" s="5" t="s">
+    <row r="27" spans="6:13" s="2" customFormat="1" ht="39.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="F27" s="26" t="s">
         <v>51</v>
       </c>
-      <c r="G27" s="6" t="s">
+      <c r="G27" s="27" t="s">
         <v>52</v>
       </c>
-      <c r="H27" s="8" t="s">
+      <c r="H27" s="28" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="28" spans="6:13" s="2" customFormat="1" ht="39.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="6:13" s="2" customFormat="1" ht="39.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="F28" s="5" t="s">
         <v>53</v>
       </c>
-      <c r="G28" s="6" t="s">
-        <v>54</v>
+      <c r="G28" s="29" t="s">
+        <v>67</v>
       </c>
       <c r="H28" s="9" t="s">
         <v>46</v>
       </c>
       <c r="I28" s="1"/>
     </row>
-    <row r="29" spans="6:13" s="2" customFormat="1" ht="39.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="F29" s="5" t="s">
+    <row r="29" spans="6:13" s="2" customFormat="1" ht="39.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="F29" s="26" t="s">
+        <v>54</v>
+      </c>
+      <c r="G29" s="27" t="s">
         <v>55</v>
       </c>
-      <c r="G29" s="6" t="s">
+      <c r="H29" s="28" t="s">
+        <v>35</v>
+      </c>
+      <c r="I29" s="1"/>
+    </row>
+    <row r="30" spans="6:13" s="2" customFormat="1" ht="39.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="F30" s="26" t="s">
         <v>56</v>
       </c>
-      <c r="H29" s="8" t="s">
-        <v>35</v>
-      </c>
-      <c r="I29" s="1"/>
-    </row>
-    <row r="30" spans="6:13" s="2" customFormat="1" ht="39.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="F30" s="5" t="s">
+      <c r="G30" s="27" t="s">
         <v>57</v>
       </c>
-      <c r="G30" s="6" t="s">
+      <c r="H30" s="28" t="s">
+        <v>46</v>
+      </c>
+      <c r="I30" s="1"/>
+    </row>
+    <row r="31" spans="6:13" s="2" customFormat="1" ht="39.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="F31" s="26" t="s">
         <v>58</v>
       </c>
-      <c r="H30" s="9" t="s">
+      <c r="G31" s="27" t="s">
+        <v>59</v>
+      </c>
+      <c r="H31" s="28" t="s">
         <v>46</v>
       </c>
-      <c r="I30" s="1"/>
-    </row>
-    <row r="31" spans="6:13" s="2" customFormat="1" ht="39.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="F31" s="5" t="s">
-        <v>59</v>
-      </c>
-      <c r="G31" s="6" t="s">
+      <c r="I31" s="1"/>
+    </row>
+    <row r="32" spans="6:13" s="2" customFormat="1" ht="39.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="F32" s="5" t="s">
         <v>60</v>
       </c>
-      <c r="H31" s="9" t="s">
+      <c r="G32" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="H32" s="22" t="s">
         <v>46</v>
       </c>
-      <c r="I31" s="1"/>
-    </row>
-    <row r="32" spans="6:13" s="2" customFormat="1" ht="39.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="F32" s="5" t="s">
-        <v>61</v>
-      </c>
-      <c r="G32" s="5" t="s">
+      <c r="I32" s="1"/>
+    </row>
+    <row r="33" spans="6:9" s="2" customFormat="1" ht="39.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="F33" s="5" t="s">
         <v>62</v>
       </c>
-      <c r="H32" s="9" t="s">
-        <v>46</v>
-      </c>
-      <c r="I32" s="1"/>
-    </row>
-    <row r="33" spans="6:9" s="2" customFormat="1" ht="39.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="F33" s="5" t="s">
+      <c r="G33" s="5" t="s">
         <v>63</v>
-      </c>
-      <c r="G33" s="5" t="s">
-        <v>64</v>
       </c>
       <c r="H33" s="9" t="s">
         <v>46</v>
       </c>
       <c r="I33" s="1"/>
     </row>
-    <row r="34" spans="6:9" s="2" customFormat="1" ht="39.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="34" spans="6:9" s="2" customFormat="1" ht="39.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="F34" s="5" t="s">
-        <v>65</v>
-      </c>
-      <c r="G34" s="5" t="s">
-        <v>66</v>
+        <v>64</v>
+      </c>
+      <c r="G34" s="30" t="s">
+        <v>68</v>
       </c>
       <c r="H34" s="9" t="s">
         <v>46</v>
       </c>
       <c r="I34" s="1"/>
     </row>
-    <row r="35" spans="6:9" s="2" customFormat="1" ht="35.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="35" spans="6:9" s="2" customFormat="1" ht="35.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="F35" s="1"/>
       <c r="G35" s="1"/>
       <c r="H35" s="10"/>
       <c r="I35" s="1"/>
     </row>
-    <row r="36" spans="6:9" s="2" customFormat="1" ht="35.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="36" spans="6:9" s="2" customFormat="1" ht="35.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="F36" s="1"/>
       <c r="G36" s="1"/>
       <c r="H36" s="10"/>
       <c r="I36" s="1"/>
     </row>
-    <row r="37" spans="6:9" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="37" spans="6:9" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="F37" s="1"/>
       <c r="G37" s="1"/>
       <c r="H37" s="10"/>
       <c r="I37" s="1"/>
     </row>
-    <row r="38" spans="6:9" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="38" spans="6:9" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="F38" s="1"/>
       <c r="G38" s="1"/>
       <c r="H38" s="10"/>
       <c r="I38" s="1"/>
     </row>
-    <row r="39" spans="6:9" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="39" spans="6:9" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="F39" s="1"/>
       <c r="G39" s="1"/>
       <c r="H39" s="10"/>
       <c r="I39" s="1"/>
     </row>
-    <row r="40" spans="6:9" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="40" spans="6:9" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="F40" s="1"/>
       <c r="G40" s="1"/>
       <c r="H40" s="10"/>
       <c r="I40" s="1"/>
     </row>
-    <row r="41" spans="6:9" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="41" spans="6:9" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="F41" s="1"/>
       <c r="G41" s="1"/>
       <c r="H41" s="10"/>
       <c r="I41" s="1"/>
     </row>
-    <row r="42" spans="6:9" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="42" spans="6:9" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="F42" s="1"/>
       <c r="G42" s="1"/>
       <c r="H42" s="10"/>
       <c r="I42" s="1"/>
     </row>
-    <row r="43" spans="6:9" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="43" spans="6:9" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="F43" s="1"/>
       <c r="G43" s="1"/>
       <c r="H43" s="10"/>
       <c r="I43" s="1"/>
     </row>
-    <row r="44" spans="6:9" ht="50.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="44" spans="6:9" ht="50.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="F44" s="1"/>
       <c r="G44" s="1"/>
       <c r="H44" s="10"/>
       <c r="I44" s="1"/>
     </row>
-    <row r="45" spans="6:9" ht="50.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="45" spans="6:9" ht="50.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="F45" s="1"/>
       <c r="G45" s="1"/>
       <c r="H45" s="10"/>
       <c r="I45" s="1"/>
     </row>
-    <row r="46" spans="6:9" ht="50.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="46" spans="6:9" ht="50.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="F46" s="1"/>
       <c r="G46" s="1"/>
       <c r="H46" s="10"/>
       <c r="I46" s="1"/>
     </row>
-    <row r="47" spans="6:9" ht="50.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="47" spans="6:9" ht="50.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="F47" s="1"/>
       <c r="G47" s="1"/>
       <c r="H47" s="10"/>
       <c r="I47" s="1"/>
     </row>
-    <row r="48" spans="6:9" ht="50.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="49" spans="13:13" ht="50.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="50" spans="13:13" ht="50.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="51" spans="13:13" ht="50.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="52" spans="13:13" ht="50.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="48" spans="6:9" ht="50.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="49" spans="13:13" ht="50.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="50" spans="13:13" ht="50.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="51" spans="13:13" ht="50.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="52" spans="13:13" ht="50.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="M52" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="53" spans="13:13" ht="50.25" customHeight="1" x14ac:dyDescent="0.3"/>
+        <v>65</v>
+      </c>
+    </row>
+    <row r="53" spans="13:13" ht="50.25" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="F2:H2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Documento Sprint-Review (03/10) doc.wrd
</commit_message>
<xml_diff>
--- a/Documentacao/Backlog.xlsx
+++ b/Documentacao/Backlog.xlsx
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="281" uniqueCount="111">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="281" uniqueCount="112">
   <si>
     <t>Projeto Umi - Backlog</t>
   </si>
@@ -372,6 +372,9 @@
   </si>
   <si>
     <t>SP2</t>
+  </si>
+  <si>
+    <t>Diagrama de Solução</t>
   </si>
 </sst>
 </file>
@@ -748,12 +751,6 @@
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -769,6 +766,37 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="14" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -778,13 +806,7 @@
     <xf numFmtId="0" fontId="14" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -793,25 +815,6 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1236,8 +1239,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="D2:N160"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="B2" zoomScale="40" zoomScaleNormal="40" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="B1" zoomScale="40" zoomScaleNormal="40" workbookViewId="0">
+      <selection activeCell="F30" sqref="F30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.45"/>
@@ -1258,17 +1261,17 @@
   </cols>
   <sheetData>
     <row r="2" spans="6:14" ht="67.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="F2" s="24" t="s">
+      <c r="F2" s="38" t="s">
         <v>0</v>
       </c>
-      <c r="G2" s="25"/>
-      <c r="H2" s="25"/>
-      <c r="I2" s="25"/>
-      <c r="J2" s="25"/>
-      <c r="K2" s="25"/>
-      <c r="L2" s="25"/>
-      <c r="M2" s="25"/>
-      <c r="N2" s="25"/>
+      <c r="G2" s="39"/>
+      <c r="H2" s="39"/>
+      <c r="I2" s="39"/>
+      <c r="J2" s="39"/>
+      <c r="K2" s="39"/>
+      <c r="L2" s="39"/>
+      <c r="M2" s="39"/>
+      <c r="N2" s="39"/>
     </row>
     <row r="3" spans="6:14" s="5" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="F3" s="4"/>
@@ -2022,7 +2025,7 @@
     </row>
     <row r="39" spans="4:14" s="7" customFormat="1" ht="39.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="F39" s="10" t="s">
-        <v>76</v>
+        <v>111</v>
       </c>
       <c r="G39" s="10" t="s">
         <v>77</v>
@@ -3512,7 +3515,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I241"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+    <sheetView showGridLines="0" topLeftCell="A3" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
       <selection activeCell="H6" sqref="H6"/>
     </sheetView>
   </sheetViews>
@@ -3526,30 +3529,30 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="56" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A1" s="33" t="s">
+      <c r="A1" s="42" t="s">
         <v>98</v>
       </c>
-      <c r="B1" s="34"/>
-      <c r="C1" s="34"/>
-      <c r="D1" s="35"/>
-      <c r="E1" s="26"/>
+      <c r="B1" s="43"/>
+      <c r="C1" s="43"/>
+      <c r="D1" s="44"/>
+      <c r="E1" s="24"/>
     </row>
     <row r="2" spans="1:9" s="5" customFormat="1" ht="18.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A2" s="27"/>
-      <c r="B2" s="28"/>
-      <c r="C2" s="28"/>
-      <c r="D2" s="29"/>
-      <c r="E2" s="30"/>
+      <c r="A2" s="25"/>
+      <c r="B2" s="26"/>
+      <c r="C2" s="26"/>
+      <c r="D2" s="27"/>
+      <c r="E2" s="28"/>
     </row>
     <row r="3" spans="1:9" ht="39.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A3" s="36" t="s">
+      <c r="A3" s="31" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="37" t="s">
+      <c r="B3" s="45" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="37"/>
-      <c r="D3" s="38" t="s">
+      <c r="C3" s="45"/>
+      <c r="D3" s="32" t="s">
         <v>3</v>
       </c>
     </row>
@@ -3557,23 +3560,23 @@
       <c r="A4" s="10" t="s">
         <v>95</v>
       </c>
-      <c r="B4" s="39" t="s">
+      <c r="B4" s="46" t="s">
         <v>96</v>
       </c>
-      <c r="C4" s="40"/>
-      <c r="D4" s="41" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" s="31" customFormat="1" ht="39.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="C4" s="47"/>
+      <c r="D4" s="33" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" s="29" customFormat="1" ht="39.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A5" s="10" t="s">
         <v>66</v>
       </c>
-      <c r="B5" s="39" t="s">
+      <c r="B5" s="46" t="s">
         <v>67</v>
       </c>
-      <c r="C5" s="40"/>
-      <c r="D5" s="42" t="s">
+      <c r="C5" s="47"/>
+      <c r="D5" s="34" t="s">
         <v>6</v>
       </c>
     </row>
@@ -3581,11 +3584,11 @@
       <c r="A6" s="10" t="s">
         <v>68</v>
       </c>
-      <c r="B6" s="43" t="s">
+      <c r="B6" s="40" t="s">
         <v>69</v>
       </c>
-      <c r="C6" s="44"/>
-      <c r="D6" s="42" t="s">
+      <c r="C6" s="41"/>
+      <c r="D6" s="34" t="s">
         <v>6</v>
       </c>
     </row>
@@ -3593,11 +3596,11 @@
       <c r="A7" s="10" t="s">
         <v>70</v>
       </c>
-      <c r="B7" s="43" t="s">
+      <c r="B7" s="40" t="s">
         <v>71</v>
       </c>
-      <c r="C7" s="44"/>
-      <c r="D7" s="42" t="s">
+      <c r="C7" s="41"/>
+      <c r="D7" s="34" t="s">
         <v>6</v>
       </c>
     </row>
@@ -3605,11 +3608,11 @@
       <c r="A8" s="10" t="s">
         <v>72</v>
       </c>
-      <c r="B8" s="43" t="s">
+      <c r="B8" s="40" t="s">
         <v>73</v>
       </c>
-      <c r="C8" s="44"/>
-      <c r="D8" s="42" t="s">
+      <c r="C8" s="41"/>
+      <c r="D8" s="34" t="s">
         <v>6</v>
       </c>
     </row>
@@ -3617,24 +3620,24 @@
       <c r="A9" s="10" t="s">
         <v>74</v>
       </c>
-      <c r="B9" s="43" t="s">
+      <c r="B9" s="40" t="s">
         <v>75</v>
       </c>
-      <c r="C9" s="44"/>
-      <c r="D9" s="42" t="s">
-        <v>6</v>
-      </c>
-      <c r="I9" s="32"/>
+      <c r="C9" s="41"/>
+      <c r="D9" s="34" t="s">
+        <v>6</v>
+      </c>
+      <c r="I9" s="30"/>
     </row>
     <row r="10" spans="1:9" ht="39.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A10" s="10" t="s">
         <v>76</v>
       </c>
-      <c r="B10" s="43" t="s">
+      <c r="B10" s="40" t="s">
         <v>77</v>
       </c>
-      <c r="C10" s="44"/>
-      <c r="D10" s="42" t="s">
+      <c r="C10" s="41"/>
+      <c r="D10" s="34" t="s">
         <v>6</v>
       </c>
     </row>
@@ -3642,11 +3645,11 @@
       <c r="A11" s="10" t="s">
         <v>78</v>
       </c>
-      <c r="B11" s="43" t="s">
+      <c r="B11" s="40" t="s">
         <v>79</v>
       </c>
-      <c r="C11" s="44"/>
-      <c r="D11" s="42" t="s">
+      <c r="C11" s="41"/>
+      <c r="D11" s="34" t="s">
         <v>6</v>
       </c>
     </row>
@@ -3654,11 +3657,11 @@
       <c r="A12" s="10" t="s">
         <v>80</v>
       </c>
-      <c r="B12" s="43" t="s">
+      <c r="B12" s="40" t="s">
         <v>81</v>
       </c>
-      <c r="C12" s="44"/>
-      <c r="D12" s="42" t="s">
+      <c r="C12" s="41"/>
+      <c r="D12" s="34" t="s">
         <v>6</v>
       </c>
     </row>
@@ -3666,11 +3669,11 @@
       <c r="A13" s="10" t="s">
         <v>97</v>
       </c>
-      <c r="B13" s="43" t="s">
+      <c r="B13" s="40" t="s">
         <v>82</v>
       </c>
-      <c r="C13" s="44"/>
-      <c r="D13" s="42" t="s">
+      <c r="C13" s="41"/>
+      <c r="D13" s="34" t="s">
         <v>6</v>
       </c>
     </row>
@@ -3678,11 +3681,11 @@
       <c r="A14" s="10" t="s">
         <v>83</v>
       </c>
-      <c r="B14" s="43" t="s">
+      <c r="B14" s="40" t="s">
         <v>84</v>
       </c>
-      <c r="C14" s="44"/>
-      <c r="D14" s="42" t="s">
+      <c r="C14" s="41"/>
+      <c r="D14" s="34" t="s">
         <v>6</v>
       </c>
     </row>
@@ -3690,11 +3693,11 @@
       <c r="A15" s="10" t="s">
         <v>85</v>
       </c>
-      <c r="B15" s="43" t="s">
+      <c r="B15" s="40" t="s">
         <v>86</v>
       </c>
-      <c r="C15" s="44"/>
-      <c r="D15" s="42" t="s">
+      <c r="C15" s="41"/>
+      <c r="D15" s="34" t="s">
         <v>6</v>
       </c>
     </row>
@@ -3702,11 +3705,11 @@
       <c r="A16" s="10" t="s">
         <v>87</v>
       </c>
-      <c r="B16" s="43" t="s">
+      <c r="B16" s="40" t="s">
         <v>88</v>
       </c>
-      <c r="C16" s="44"/>
-      <c r="D16" s="42" t="s">
+      <c r="C16" s="41"/>
+      <c r="D16" s="34" t="s">
         <v>6</v>
       </c>
     </row>
@@ -3714,11 +3717,11 @@
       <c r="A17" s="10" t="s">
         <v>89</v>
       </c>
-      <c r="B17" s="43" t="s">
+      <c r="B17" s="40" t="s">
         <v>90</v>
       </c>
-      <c r="C17" s="44"/>
-      <c r="D17" s="42" t="s">
+      <c r="C17" s="41"/>
+      <c r="D17" s="34" t="s">
         <v>6</v>
       </c>
     </row>
@@ -3726,233 +3729,233 @@
       <c r="A18" s="10" t="s">
         <v>91</v>
       </c>
-      <c r="B18" s="43" t="s">
+      <c r="B18" s="40" t="s">
         <v>92</v>
       </c>
-      <c r="C18" s="44"/>
-      <c r="D18" s="42" t="s">
+      <c r="C18" s="41"/>
+      <c r="D18" s="34" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="19" spans="1:4" ht="39.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A19" s="10"/>
-      <c r="B19" s="43"/>
-      <c r="C19" s="44"/>
-      <c r="D19" s="45"/>
+      <c r="B19" s="40"/>
+      <c r="C19" s="41"/>
+      <c r="D19" s="35"/>
     </row>
     <row r="20" spans="1:4" ht="39.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A20" s="10"/>
-      <c r="B20" s="43"/>
-      <c r="C20" s="44"/>
-      <c r="D20" s="45"/>
+      <c r="B20" s="40"/>
+      <c r="C20" s="41"/>
+      <c r="D20" s="35"/>
     </row>
     <row r="21" spans="1:4" ht="39.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A21" s="10"/>
-      <c r="B21" s="43"/>
-      <c r="C21" s="44"/>
-      <c r="D21" s="45"/>
+      <c r="B21" s="40"/>
+      <c r="C21" s="41"/>
+      <c r="D21" s="35"/>
     </row>
     <row r="22" spans="1:4" ht="39.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A22" s="10"/>
-      <c r="B22" s="43"/>
-      <c r="C22" s="44"/>
-      <c r="D22" s="45"/>
+      <c r="B22" s="40"/>
+      <c r="C22" s="41"/>
+      <c r="D22" s="35"/>
     </row>
     <row r="23" spans="1:4" ht="39.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A23" s="10"/>
-      <c r="B23" s="43"/>
-      <c r="C23" s="44"/>
-      <c r="D23" s="45"/>
+      <c r="B23" s="40"/>
+      <c r="C23" s="41"/>
+      <c r="D23" s="35"/>
     </row>
     <row r="24" spans="1:4" ht="39.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A24" s="10"/>
-      <c r="B24" s="43"/>
-      <c r="C24" s="44"/>
-      <c r="D24" s="46"/>
+      <c r="B24" s="40"/>
+      <c r="C24" s="41"/>
+      <c r="D24" s="36"/>
     </row>
     <row r="25" spans="1:4" ht="39.75" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A25" s="21"/>
-      <c r="B25" s="47"/>
-      <c r="C25" s="47"/>
+      <c r="B25" s="37"/>
+      <c r="C25" s="37"/>
       <c r="D25" s="21"/>
     </row>
     <row r="26" spans="1:4" ht="39.75" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A26" s="21"/>
-      <c r="B26" s="47"/>
-      <c r="C26" s="47"/>
+      <c r="B26" s="37"/>
+      <c r="C26" s="37"/>
       <c r="D26" s="21"/>
     </row>
     <row r="27" spans="1:4" ht="39.75" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A27" s="21"/>
-      <c r="B27" s="47"/>
-      <c r="C27" s="47"/>
+      <c r="B27" s="37"/>
+      <c r="C27" s="37"/>
       <c r="D27" s="21"/>
     </row>
     <row r="28" spans="1:4" ht="39.75" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A28" s="21"/>
-      <c r="B28" s="47"/>
-      <c r="C28" s="47"/>
+      <c r="B28" s="37"/>
+      <c r="C28" s="37"/>
       <c r="D28" s="21"/>
     </row>
     <row r="29" spans="1:4" ht="39.75" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A29" s="21"/>
-      <c r="B29" s="47"/>
-      <c r="C29" s="47"/>
+      <c r="B29" s="37"/>
+      <c r="C29" s="37"/>
       <c r="D29" s="21"/>
     </row>
     <row r="30" spans="1:4" ht="39.75" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A30" s="21"/>
-      <c r="B30" s="47"/>
-      <c r="C30" s="47"/>
+      <c r="B30" s="37"/>
+      <c r="C30" s="37"/>
       <c r="D30" s="21"/>
     </row>
     <row r="31" spans="1:4" ht="39.75" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A31" s="21"/>
-      <c r="B31" s="47"/>
-      <c r="C31" s="47"/>
+      <c r="B31" s="37"/>
+      <c r="C31" s="37"/>
       <c r="D31" s="21"/>
     </row>
     <row r="32" spans="1:4" ht="39.75" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A32" s="21"/>
-      <c r="B32" s="47"/>
-      <c r="C32" s="47"/>
+      <c r="B32" s="37"/>
+      <c r="C32" s="37"/>
       <c r="D32" s="21"/>
     </row>
     <row r="33" spans="1:4" ht="39.75" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A33" s="21"/>
-      <c r="B33" s="47"/>
-      <c r="C33" s="47"/>
+      <c r="B33" s="37"/>
+      <c r="C33" s="37"/>
       <c r="D33" s="21"/>
     </row>
     <row r="34" spans="1:4" ht="39.75" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A34" s="21"/>
-      <c r="B34" s="47"/>
-      <c r="C34" s="47"/>
+      <c r="B34" s="37"/>
+      <c r="C34" s="37"/>
       <c r="D34" s="21"/>
     </row>
     <row r="35" spans="1:4" ht="39.75" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A35" s="21"/>
-      <c r="B35" s="47"/>
-      <c r="C35" s="47"/>
+      <c r="B35" s="37"/>
+      <c r="C35" s="37"/>
       <c r="D35" s="21"/>
     </row>
     <row r="36" spans="1:4" ht="39.75" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A36" s="21"/>
-      <c r="B36" s="47"/>
-      <c r="C36" s="47"/>
+      <c r="B36" s="37"/>
+      <c r="C36" s="37"/>
       <c r="D36" s="21"/>
     </row>
     <row r="37" spans="1:4" ht="39.75" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A37" s="21"/>
-      <c r="B37" s="47"/>
-      <c r="C37" s="47"/>
+      <c r="B37" s="37"/>
+      <c r="C37" s="37"/>
       <c r="D37" s="21"/>
     </row>
     <row r="38" spans="1:4" ht="39.75" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A38" s="21"/>
-      <c r="B38" s="47"/>
-      <c r="C38" s="47"/>
+      <c r="B38" s="37"/>
+      <c r="C38" s="37"/>
       <c r="D38" s="21"/>
     </row>
     <row r="39" spans="1:4" ht="39.75" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A39" s="21"/>
-      <c r="B39" s="47"/>
-      <c r="C39" s="47"/>
+      <c r="B39" s="37"/>
+      <c r="C39" s="37"/>
       <c r="D39" s="21"/>
     </row>
     <row r="40" spans="1:4" ht="39.75" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A40" s="21"/>
-      <c r="B40" s="47"/>
-      <c r="C40" s="47"/>
+      <c r="B40" s="37"/>
+      <c r="C40" s="37"/>
       <c r="D40" s="21"/>
     </row>
     <row r="41" spans="1:4" ht="39.75" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B41" s="26"/>
-      <c r="C41" s="26"/>
+      <c r="B41" s="24"/>
+      <c r="C41" s="24"/>
     </row>
     <row r="42" spans="1:4" ht="39.75" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B42" s="26"/>
-      <c r="C42" s="26"/>
+      <c r="B42" s="24"/>
+      <c r="C42" s="24"/>
     </row>
     <row r="43" spans="1:4" ht="39.75" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B43" s="26"/>
-      <c r="C43" s="26"/>
+      <c r="B43" s="24"/>
+      <c r="C43" s="24"/>
     </row>
     <row r="44" spans="1:4" ht="39.75" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B44" s="26"/>
-      <c r="C44" s="26"/>
+      <c r="B44" s="24"/>
+      <c r="C44" s="24"/>
     </row>
     <row r="45" spans="1:4" ht="39.75" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B45" s="26"/>
-      <c r="C45" s="26"/>
+      <c r="B45" s="24"/>
+      <c r="C45" s="24"/>
     </row>
     <row r="46" spans="1:4" ht="39.75" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B46" s="26"/>
-      <c r="C46" s="26"/>
+      <c r="B46" s="24"/>
+      <c r="C46" s="24"/>
     </row>
     <row r="47" spans="1:4" ht="39.75" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B47" s="26"/>
-      <c r="C47" s="26"/>
+      <c r="B47" s="24"/>
+      <c r="C47" s="24"/>
     </row>
     <row r="48" spans="1:4" ht="39.75" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B48" s="26"/>
-      <c r="C48" s="26"/>
+      <c r="B48" s="24"/>
+      <c r="C48" s="24"/>
     </row>
     <row r="49" spans="2:3" ht="39.75" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B49" s="26"/>
-      <c r="C49" s="26"/>
+      <c r="B49" s="24"/>
+      <c r="C49" s="24"/>
     </row>
     <row r="50" spans="2:3" ht="39.75" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B50" s="26"/>
-      <c r="C50" s="26"/>
+      <c r="B50" s="24"/>
+      <c r="C50" s="24"/>
     </row>
     <row r="51" spans="2:3" ht="39.75" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B51" s="26"/>
-      <c r="C51" s="26"/>
+      <c r="B51" s="24"/>
+      <c r="C51" s="24"/>
     </row>
     <row r="52" spans="2:3" ht="39.75" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B52" s="26"/>
-      <c r="C52" s="26"/>
+      <c r="B52" s="24"/>
+      <c r="C52" s="24"/>
     </row>
     <row r="53" spans="2:3" ht="39.75" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B53" s="26"/>
-      <c r="C53" s="26"/>
+      <c r="B53" s="24"/>
+      <c r="C53" s="24"/>
     </row>
     <row r="54" spans="2:3" ht="39.75" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B54" s="26"/>
-      <c r="C54" s="26"/>
+      <c r="B54" s="24"/>
+      <c r="C54" s="24"/>
     </row>
     <row r="55" spans="2:3" ht="39.75" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B55" s="26"/>
-      <c r="C55" s="26"/>
+      <c r="B55" s="24"/>
+      <c r="C55" s="24"/>
     </row>
     <row r="56" spans="2:3" ht="39.75" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B56" s="26"/>
-      <c r="C56" s="26"/>
+      <c r="B56" s="24"/>
+      <c r="C56" s="24"/>
     </row>
     <row r="57" spans="2:3" ht="39.75" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B57" s="26"/>
-      <c r="C57" s="26"/>
+      <c r="B57" s="24"/>
+      <c r="C57" s="24"/>
     </row>
     <row r="58" spans="2:3" ht="39.75" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B58" s="26"/>
-      <c r="C58" s="26"/>
+      <c r="B58" s="24"/>
+      <c r="C58" s="24"/>
     </row>
     <row r="59" spans="2:3" ht="39.75" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B59" s="26"/>
-      <c r="C59" s="26"/>
+      <c r="B59" s="24"/>
+      <c r="C59" s="24"/>
     </row>
     <row r="60" spans="2:3" ht="39.75" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B60" s="26"/>
-      <c r="C60" s="26"/>
+      <c r="B60" s="24"/>
+      <c r="C60" s="24"/>
     </row>
     <row r="61" spans="2:3" ht="39.75" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B61" s="26"/>
-      <c r="C61" s="26"/>
+      <c r="B61" s="24"/>
+      <c r="C61" s="24"/>
     </row>
     <row r="62" spans="2:3" ht="39.75" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B62" s="26"/>
-      <c r="C62" s="26"/>
+      <c r="B62" s="24"/>
+      <c r="C62" s="24"/>
     </row>
     <row r="63" spans="2:3" ht="39.75" customHeight="1" x14ac:dyDescent="0.45"/>
     <row r="64" spans="2:3" ht="39.75" customHeight="1" x14ac:dyDescent="0.45"/>
@@ -4135,12 +4138,11 @@
     <row r="241" ht="39.75" customHeight="1" x14ac:dyDescent="0.45"/>
   </sheetData>
   <mergeCells count="23">
-    <mergeCell ref="B7:C7"/>
-    <mergeCell ref="A1:D1"/>
-    <mergeCell ref="B3:C3"/>
-    <mergeCell ref="B4:C4"/>
-    <mergeCell ref="B5:C5"/>
-    <mergeCell ref="B6:C6"/>
+    <mergeCell ref="B20:C20"/>
+    <mergeCell ref="B21:C21"/>
+    <mergeCell ref="B22:C22"/>
+    <mergeCell ref="B23:C23"/>
+    <mergeCell ref="B24:C24"/>
     <mergeCell ref="B19:C19"/>
     <mergeCell ref="B8:C8"/>
     <mergeCell ref="B9:C9"/>
@@ -4153,11 +4155,12 @@
     <mergeCell ref="B16:C16"/>
     <mergeCell ref="B17:C17"/>
     <mergeCell ref="B18:C18"/>
-    <mergeCell ref="B20:C20"/>
-    <mergeCell ref="B21:C21"/>
-    <mergeCell ref="B22:C22"/>
-    <mergeCell ref="B23:C23"/>
-    <mergeCell ref="B24:C24"/>
+    <mergeCell ref="B7:C7"/>
+    <mergeCell ref="A1:D1"/>
+    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="B4:C4"/>
+    <mergeCell ref="B5:C5"/>
+    <mergeCell ref="B6:C6"/>
   </mergeCells>
   <conditionalFormatting sqref="C2">
     <cfRule type="containsText" dxfId="2" priority="1" operator="containsText" text="Desejável">

</xml_diff>

<commit_message>
Update: inserção do planejamento semanal e alteração na documentação do projeto
</commit_message>
<xml_diff>
--- a/Documentacao/Backlog.xlsx
+++ b/Documentacao/Backlog.xlsx
@@ -5,18 +5,18 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Admin\Desktop\Repositório-UMITRIX\UMITRIX\Documentacao\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\supor\Documents\Faculdade\PI\Projeto-SPTech\UMITRIX\Documentacao\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="2340" yWindow="2340" windowWidth="18000" windowHeight="9810"/>
+    <workbookView xWindow="2340" yWindow="2340" windowWidth="18000" windowHeight="9816"/>
   </bookViews>
   <sheets>
     <sheet name="Backlog" sheetId="1" r:id="rId1"/>
     <sheet name="Backlog S-2" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Backlog!$F$4:$N$4</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Backlog!$F$4:$N$39</definedName>
   </definedNames>
   <calcPr calcId="162913"/>
   <extLst>
@@ -700,6 +700,21 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -729,21 +744,6 @@
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1169,41 +1169,41 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="D2:N149"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="C1" zoomScale="36" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="D1" zoomScale="50" zoomScaleNormal="50" workbookViewId="0">
+      <selection activeCell="J10" sqref="J10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultColWidth="8.69921875" defaultRowHeight="16.8" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="3" width="8.6640625" style="1"/>
+    <col min="1" max="3" width="8.69921875" style="1"/>
     <col min="4" max="4" width="12.5" style="1" customWidth="1"/>
-    <col min="5" max="5" width="12.58203125" style="1" customWidth="1"/>
-    <col min="6" max="6" width="57.9140625" style="1" customWidth="1"/>
-    <col min="7" max="7" width="141.75" style="1" customWidth="1"/>
-    <col min="8" max="8" width="27.4140625" style="2" customWidth="1"/>
-    <col min="9" max="9" width="19.4140625" style="3" customWidth="1"/>
+    <col min="5" max="5" width="12.59765625" style="1" customWidth="1"/>
+    <col min="6" max="6" width="57.8984375" style="1" customWidth="1"/>
+    <col min="7" max="7" width="141.69921875" style="1" customWidth="1"/>
+    <col min="8" max="8" width="27.3984375" style="2" customWidth="1"/>
+    <col min="9" max="9" width="19.3984375" style="3" customWidth="1"/>
     <col min="10" max="10" width="15" style="3" customWidth="1"/>
-    <col min="11" max="11" width="21.33203125" style="3" customWidth="1"/>
-    <col min="12" max="12" width="15.1640625" style="3" customWidth="1"/>
-    <col min="13" max="13" width="18.75" style="3" customWidth="1"/>
+    <col min="11" max="11" width="21.296875" style="3" customWidth="1"/>
+    <col min="12" max="12" width="15.19921875" style="3" customWidth="1"/>
+    <col min="13" max="13" width="18.69921875" style="3" customWidth="1"/>
     <col min="14" max="14" width="25.5" style="1" customWidth="1"/>
-    <col min="15" max="16384" width="8.6640625" style="1"/>
+    <col min="15" max="16384" width="8.69921875" style="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="6:14" ht="67.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="F2" s="29" t="s">
+    <row r="2" spans="6:14" ht="67.5" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="F2" s="34" t="s">
         <v>84</v>
       </c>
-      <c r="G2" s="30"/>
-      <c r="H2" s="30"/>
-      <c r="I2" s="30"/>
-      <c r="J2" s="30"/>
-      <c r="K2" s="30"/>
-      <c r="L2" s="30"/>
-      <c r="M2" s="30"/>
-      <c r="N2" s="30"/>
-    </row>
-    <row r="3" spans="6:14" s="5" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="G2" s="35"/>
+      <c r="H2" s="35"/>
+      <c r="I2" s="35"/>
+      <c r="J2" s="35"/>
+      <c r="K2" s="35"/>
+      <c r="L2" s="35"/>
+      <c r="M2" s="35"/>
+      <c r="N2" s="35"/>
+    </row>
+    <row r="3" spans="6:14" s="5" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.4">
       <c r="F3" s="4"/>
       <c r="G3" s="4"/>
       <c r="H3" s="4"/>
@@ -1213,7 +1213,7 @@
       <c r="L3" s="6"/>
       <c r="M3" s="6"/>
     </row>
-    <row r="4" spans="6:14" s="2" customFormat="1" ht="36" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="6:14" s="2" customFormat="1" ht="36" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="F4" s="9" t="s">
         <v>0</v>
       </c>
@@ -1242,7 +1242,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="5" spans="6:14" s="7" customFormat="1" ht="39.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="6:14" s="7" customFormat="1" ht="39.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="F5" s="10" t="s">
         <v>3</v>
       </c>
@@ -1269,7 +1269,7 @@
       </c>
       <c r="N5" s="11"/>
     </row>
-    <row r="6" spans="6:14" s="7" customFormat="1" ht="39.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="6:14" s="7" customFormat="1" ht="39.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="F6" s="10" t="s">
         <v>6</v>
       </c>
@@ -1296,7 +1296,7 @@
       </c>
       <c r="N6" s="11"/>
     </row>
-    <row r="7" spans="6:14" s="7" customFormat="1" ht="39.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="6:14" s="7" customFormat="1" ht="39.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="F7" s="10" t="s">
         <v>8</v>
       </c>
@@ -1323,7 +1323,7 @@
       </c>
       <c r="N7" s="11"/>
     </row>
-    <row r="8" spans="6:14" s="7" customFormat="1" ht="39.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="6:14" s="7" customFormat="1" ht="39.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="F8" s="10" t="s">
         <v>10</v>
       </c>
@@ -1350,7 +1350,7 @@
       </c>
       <c r="N8" s="11"/>
     </row>
-    <row r="9" spans="6:14" s="7" customFormat="1" ht="39.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="6:14" s="7" customFormat="1" ht="39.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="F9" s="10" t="s">
         <v>12</v>
       </c>
@@ -1377,7 +1377,7 @@
       </c>
       <c r="N9" s="11"/>
     </row>
-    <row r="10" spans="6:14" s="7" customFormat="1" ht="39.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="6:14" s="7" customFormat="1" ht="39.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="F10" s="10" t="s">
         <v>14</v>
       </c>
@@ -1404,7 +1404,7 @@
       </c>
       <c r="N10" s="11"/>
     </row>
-    <row r="11" spans="6:14" s="7" customFormat="1" ht="39.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="11" spans="6:14" s="7" customFormat="1" ht="39.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="F11" s="10" t="s">
         <v>16</v>
       </c>
@@ -1431,7 +1431,7 @@
       </c>
       <c r="N11" s="11"/>
     </row>
-    <row r="12" spans="6:14" s="7" customFormat="1" ht="39.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="12" spans="6:14" s="7" customFormat="1" ht="39.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="F12" s="10" t="s">
         <v>18</v>
       </c>
@@ -1458,7 +1458,7 @@
       </c>
       <c r="N12" s="11"/>
     </row>
-    <row r="13" spans="6:14" s="7" customFormat="1" ht="39.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="13" spans="6:14" s="7" customFormat="1" ht="39.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="F13" s="10" t="s">
         <v>20</v>
       </c>
@@ -1485,7 +1485,7 @@
       </c>
       <c r="N13" s="11"/>
     </row>
-    <row r="14" spans="6:14" s="7" customFormat="1" ht="39.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="14" spans="6:14" s="7" customFormat="1" ht="39.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="F14" s="10" t="s">
         <v>22</v>
       </c>
@@ -1512,7 +1512,7 @@
       </c>
       <c r="N14" s="11"/>
     </row>
-    <row r="15" spans="6:14" s="7" customFormat="1" ht="39.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="15" spans="6:14" s="7" customFormat="1" ht="39.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="F15" s="10" t="s">
         <v>24</v>
       </c>
@@ -1539,7 +1539,7 @@
       </c>
       <c r="N15" s="11"/>
     </row>
-    <row r="16" spans="6:14" s="7" customFormat="1" ht="39.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="16" spans="6:14" s="7" customFormat="1" ht="39.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="F16" s="10" t="s">
         <v>91</v>
       </c>
@@ -1566,7 +1566,7 @@
       </c>
       <c r="N16" s="11"/>
     </row>
-    <row r="17" spans="6:14" s="7" customFormat="1" ht="39.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="17" spans="6:14" s="7" customFormat="1" ht="39.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="F17" s="10" t="s">
         <v>27</v>
       </c>
@@ -1593,7 +1593,7 @@
       </c>
       <c r="N17" s="11"/>
     </row>
-    <row r="18" spans="6:14" s="7" customFormat="1" ht="39.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="18" spans="6:14" s="7" customFormat="1" ht="39.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="F18" s="10" t="s">
         <v>30</v>
       </c>
@@ -1620,7 +1620,7 @@
       </c>
       <c r="N18" s="11"/>
     </row>
-    <row r="19" spans="6:14" s="7" customFormat="1" ht="39.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="19" spans="6:14" s="7" customFormat="1" ht="39.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="F19" s="10" t="s">
         <v>32</v>
       </c>
@@ -1647,7 +1647,7 @@
       </c>
       <c r="N19" s="11"/>
     </row>
-    <row r="20" spans="6:14" s="7" customFormat="1" ht="39.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="20" spans="6:14" s="7" customFormat="1" ht="39.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="F20" s="10" t="s">
         <v>92</v>
       </c>
@@ -1674,7 +1674,7 @@
       </c>
       <c r="N20" s="11"/>
     </row>
-    <row r="21" spans="6:14" s="7" customFormat="1" ht="39.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="21" spans="6:14" s="7" customFormat="1" ht="39.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="F21" s="10" t="s">
         <v>94</v>
       </c>
@@ -1701,7 +1701,7 @@
       </c>
       <c r="N21" s="11"/>
     </row>
-    <row r="22" spans="6:14" s="7" customFormat="1" ht="39.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="22" spans="6:14" s="7" customFormat="1" ht="39.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="F22" s="10" t="s">
         <v>95</v>
       </c>
@@ -1728,7 +1728,7 @@
       </c>
       <c r="N22" s="11"/>
     </row>
-    <row r="23" spans="6:14" s="7" customFormat="1" ht="39.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="23" spans="6:14" s="7" customFormat="1" ht="39.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="F23" s="10" t="s">
         <v>37</v>
       </c>
@@ -1755,7 +1755,7 @@
       </c>
       <c r="N23" s="11"/>
     </row>
-    <row r="24" spans="6:14" s="7" customFormat="1" ht="39.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="24" spans="6:14" s="7" customFormat="1" ht="39.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="F24" s="10" t="s">
         <v>40</v>
       </c>
@@ -1782,7 +1782,7 @@
       </c>
       <c r="N24" s="11"/>
     </row>
-    <row r="25" spans="6:14" s="7" customFormat="1" ht="39.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="25" spans="6:14" s="7" customFormat="1" ht="39.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="F25" s="10" t="s">
         <v>42</v>
       </c>
@@ -1809,7 +1809,7 @@
       </c>
       <c r="N25" s="11"/>
     </row>
-    <row r="26" spans="6:14" s="7" customFormat="1" ht="39.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="26" spans="6:14" s="7" customFormat="1" ht="39.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="F26" s="10" t="s">
         <v>44</v>
       </c>
@@ -1836,7 +1836,7 @@
       </c>
       <c r="N26" s="11"/>
     </row>
-    <row r="27" spans="6:14" s="7" customFormat="1" ht="39.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="27" spans="6:14" s="7" customFormat="1" ht="39.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="F27" s="10" t="s">
         <v>46</v>
       </c>
@@ -1863,7 +1863,7 @@
       </c>
       <c r="N27" s="11"/>
     </row>
-    <row r="28" spans="6:14" s="7" customFormat="1" ht="39.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="28" spans="6:14" s="7" customFormat="1" ht="39.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="F28" s="10" t="s">
         <v>48</v>
       </c>
@@ -1890,7 +1890,7 @@
       </c>
       <c r="N28" s="11"/>
     </row>
-    <row r="29" spans="6:14" s="7" customFormat="1" ht="39.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="29" spans="6:14" s="7" customFormat="1" ht="39.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="F29" s="10" t="s">
         <v>83</v>
       </c>
@@ -1917,7 +1917,7 @@
       </c>
       <c r="N29" s="11"/>
     </row>
-    <row r="30" spans="6:14" s="7" customFormat="1" ht="39.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="30" spans="6:14" s="7" customFormat="1" ht="39.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="F30" s="10" t="s">
         <v>51</v>
       </c>
@@ -1944,7 +1944,7 @@
       </c>
       <c r="N30" s="11"/>
     </row>
-    <row r="31" spans="6:14" s="7" customFormat="1" ht="39.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="31" spans="6:14" s="7" customFormat="1" ht="39.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="F31" s="10" t="s">
         <v>53</v>
       </c>
@@ -1971,7 +1971,7 @@
       </c>
       <c r="N31" s="11"/>
     </row>
-    <row r="32" spans="6:14" ht="39.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="32" spans="6:14" ht="39.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
       <c r="F32" s="10" t="s">
         <v>66</v>
       </c>
@@ -1998,7 +1998,7 @@
       </c>
       <c r="N32" s="11"/>
     </row>
-    <row r="33" spans="4:14" ht="39.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="33" spans="4:14" ht="39.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
       <c r="F33" s="10" t="s">
         <v>56</v>
       </c>
@@ -2025,7 +2025,7 @@
       </c>
       <c r="N33" s="11"/>
     </row>
-    <row r="34" spans="4:14" ht="39.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="34" spans="4:14" ht="39.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
       <c r="D34" s="8" t="s">
         <v>78</v>
       </c>
@@ -2055,7 +2055,7 @@
       </c>
       <c r="N34" s="11"/>
     </row>
-    <row r="35" spans="4:14" ht="39.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="35" spans="4:14" ht="39.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
       <c r="F35" s="10" t="s">
         <v>60</v>
       </c>
@@ -2082,7 +2082,7 @@
       </c>
       <c r="N35" s="11"/>
     </row>
-    <row r="36" spans="4:14" ht="39.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="36" spans="4:14" ht="39.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
       <c r="F36" s="10" t="s">
         <v>62</v>
       </c>
@@ -2109,7 +2109,7 @@
       </c>
       <c r="N36" s="11"/>
     </row>
-    <row r="37" spans="4:14" ht="39.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="37" spans="4:14" ht="39.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
       <c r="F37" s="10" t="s">
         <v>64</v>
       </c>
@@ -2136,7 +2136,7 @@
       </c>
       <c r="N37" s="11"/>
     </row>
-    <row r="38" spans="4:14" ht="50.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="38" spans="4:14" ht="50.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
       <c r="F38" s="10" t="s">
         <v>79</v>
       </c>
@@ -2163,7 +2163,7 @@
       </c>
       <c r="N38" s="11"/>
     </row>
-    <row r="39" spans="4:14" ht="39.75" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="39" spans="4:14" ht="39.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="F39" s="17"/>
       <c r="G39" s="17"/>
       <c r="H39" s="18"/>
@@ -2176,7 +2176,7 @@
       </c>
       <c r="N39" s="17"/>
     </row>
-    <row r="40" spans="4:14" ht="39.75" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="40" spans="4:14" ht="39.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="F40" s="17"/>
       <c r="G40" s="17"/>
       <c r="H40" s="18"/>
@@ -2187,7 +2187,7 @@
       <c r="M40" s="19"/>
       <c r="N40" s="17"/>
     </row>
-    <row r="41" spans="4:14" ht="39.75" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="41" spans="4:14" ht="39.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="F41" s="17"/>
       <c r="G41" s="17"/>
       <c r="H41" s="18"/>
@@ -2198,7 +2198,7 @@
       <c r="M41" s="19"/>
       <c r="N41" s="17"/>
     </row>
-    <row r="42" spans="4:14" ht="39.75" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="42" spans="4:14" ht="39.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="F42" s="17"/>
       <c r="G42" s="17"/>
       <c r="H42" s="18"/>
@@ -2209,7 +2209,7 @@
       <c r="M42" s="19"/>
       <c r="N42" s="17"/>
     </row>
-    <row r="43" spans="4:14" ht="39.75" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="43" spans="4:14" ht="39.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="F43" s="17"/>
       <c r="G43" s="17"/>
       <c r="H43" s="18"/>
@@ -2220,7 +2220,7 @@
       <c r="M43" s="19"/>
       <c r="N43" s="17"/>
     </row>
-    <row r="44" spans="4:14" ht="39.75" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="44" spans="4:14" ht="39.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="F44" s="17"/>
       <c r="G44" s="17"/>
       <c r="H44" s="18"/>
@@ -2231,7 +2231,7 @@
       <c r="M44" s="19"/>
       <c r="N44" s="17"/>
     </row>
-    <row r="45" spans="4:14" ht="39.75" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="45" spans="4:14" ht="39.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="F45" s="17"/>
       <c r="G45" s="17"/>
       <c r="H45" s="18"/>
@@ -2242,7 +2242,7 @@
       <c r="M45" s="19"/>
       <c r="N45" s="17"/>
     </row>
-    <row r="46" spans="4:14" ht="39.75" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="46" spans="4:14" ht="39.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="F46" s="17"/>
       <c r="G46" s="17"/>
       <c r="H46" s="18"/>
@@ -2253,7 +2253,7 @@
       <c r="M46" s="19"/>
       <c r="N46" s="17"/>
     </row>
-    <row r="47" spans="4:14" ht="39.75" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="47" spans="4:14" ht="39.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="F47" s="17"/>
       <c r="G47" s="17"/>
       <c r="H47" s="18"/>
@@ -2264,7 +2264,7 @@
       <c r="M47" s="19"/>
       <c r="N47" s="17"/>
     </row>
-    <row r="48" spans="4:14" ht="39.75" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="48" spans="4:14" ht="39.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="F48" s="17"/>
       <c r="G48" s="17"/>
       <c r="H48" s="18"/>
@@ -2275,7 +2275,7 @@
       <c r="M48" s="19"/>
       <c r="N48" s="17"/>
     </row>
-    <row r="49" spans="6:14" ht="39.75" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="49" spans="6:14" ht="39.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="F49" s="17"/>
       <c r="G49" s="17"/>
       <c r="H49" s="18"/>
@@ -2286,7 +2286,7 @@
       <c r="M49" s="19"/>
       <c r="N49" s="17"/>
     </row>
-    <row r="50" spans="6:14" ht="39.75" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="50" spans="6:14" ht="39.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="F50" s="17"/>
       <c r="G50" s="17"/>
       <c r="H50" s="18"/>
@@ -2297,7 +2297,7 @@
       <c r="M50" s="19"/>
       <c r="N50" s="17"/>
     </row>
-    <row r="51" spans="6:14" ht="39.75" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="51" spans="6:14" ht="39.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="F51" s="17"/>
       <c r="G51" s="17"/>
       <c r="H51" s="18"/>
@@ -2308,7 +2308,7 @@
       <c r="M51" s="19"/>
       <c r="N51" s="17"/>
     </row>
-    <row r="52" spans="6:14" ht="39.75" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="52" spans="6:14" ht="39.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="F52" s="17"/>
       <c r="G52" s="17"/>
       <c r="H52" s="18"/>
@@ -2319,7 +2319,7 @@
       <c r="M52" s="19"/>
       <c r="N52" s="17"/>
     </row>
-    <row r="53" spans="6:14" ht="39.75" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="53" spans="6:14" ht="39.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="F53" s="17"/>
       <c r="G53" s="17"/>
       <c r="H53" s="18"/>
@@ -2330,7 +2330,7 @@
       <c r="M53" s="19"/>
       <c r="N53" s="17"/>
     </row>
-    <row r="54" spans="6:14" ht="39.75" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="54" spans="6:14" ht="39.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="F54" s="17"/>
       <c r="G54" s="17"/>
       <c r="H54" s="18"/>
@@ -2341,7 +2341,7 @@
       <c r="M54" s="19"/>
       <c r="N54" s="17"/>
     </row>
-    <row r="55" spans="6:14" ht="39.75" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="55" spans="6:14" ht="39.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="F55" s="17"/>
       <c r="G55" s="17"/>
       <c r="H55" s="18"/>
@@ -2352,7 +2352,7 @@
       <c r="M55" s="19"/>
       <c r="N55" s="17"/>
     </row>
-    <row r="56" spans="6:14" ht="39.75" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="56" spans="6:14" ht="39.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="F56" s="17"/>
       <c r="G56" s="17"/>
       <c r="H56" s="18"/>
@@ -2363,7 +2363,7 @@
       <c r="M56" s="19"/>
       <c r="N56" s="17"/>
     </row>
-    <row r="57" spans="6:14" ht="39.75" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="57" spans="6:14" ht="39.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="F57" s="17"/>
       <c r="G57" s="17"/>
       <c r="H57" s="18"/>
@@ -2374,7 +2374,7 @@
       <c r="M57" s="19"/>
       <c r="N57" s="17"/>
     </row>
-    <row r="58" spans="6:14" ht="39.75" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="58" spans="6:14" ht="39.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="F58" s="17"/>
       <c r="G58" s="17"/>
       <c r="H58" s="18"/>
@@ -2385,7 +2385,7 @@
       <c r="M58" s="19"/>
       <c r="N58" s="17"/>
     </row>
-    <row r="59" spans="6:14" ht="39.75" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="59" spans="6:14" ht="39.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="F59" s="17"/>
       <c r="G59" s="17"/>
       <c r="H59" s="18"/>
@@ -2396,7 +2396,7 @@
       <c r="M59" s="19"/>
       <c r="N59" s="17"/>
     </row>
-    <row r="60" spans="6:14" ht="39.75" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="60" spans="6:14" ht="39.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="F60" s="17"/>
       <c r="G60" s="17"/>
       <c r="H60" s="18"/>
@@ -2407,7 +2407,7 @@
       <c r="M60" s="19"/>
       <c r="N60" s="17"/>
     </row>
-    <row r="61" spans="6:14" ht="39.75" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="61" spans="6:14" ht="39.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="F61" s="17"/>
       <c r="G61" s="17"/>
       <c r="H61" s="18"/>
@@ -2418,7 +2418,7 @@
       <c r="M61" s="19"/>
       <c r="N61" s="17"/>
     </row>
-    <row r="62" spans="6:14" ht="39.75" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="62" spans="6:14" ht="39.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="F62" s="17"/>
       <c r="G62" s="17"/>
       <c r="H62" s="18"/>
@@ -2429,7 +2429,7 @@
       <c r="M62" s="19"/>
       <c r="N62" s="17"/>
     </row>
-    <row r="63" spans="6:14" ht="39.75" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="63" spans="6:14" ht="39.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="F63" s="17"/>
       <c r="G63" s="17"/>
       <c r="H63" s="18"/>
@@ -2440,7 +2440,7 @@
       <c r="M63" s="19"/>
       <c r="N63" s="17"/>
     </row>
-    <row r="64" spans="6:14" ht="39.75" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="64" spans="6:14" ht="39.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="F64" s="17"/>
       <c r="G64" s="17"/>
       <c r="H64" s="18"/>
@@ -2451,7 +2451,7 @@
       <c r="M64" s="19"/>
       <c r="N64" s="17"/>
     </row>
-    <row r="65" spans="6:14" ht="39.75" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="65" spans="6:14" ht="39.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="F65" s="17"/>
       <c r="G65" s="17"/>
       <c r="H65" s="18"/>
@@ -2462,7 +2462,7 @@
       <c r="M65" s="19"/>
       <c r="N65" s="17"/>
     </row>
-    <row r="66" spans="6:14" ht="39.75" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="66" spans="6:14" ht="39.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="F66" s="17"/>
       <c r="G66" s="17"/>
       <c r="H66" s="18"/>
@@ -2473,7 +2473,7 @@
       <c r="M66" s="19"/>
       <c r="N66" s="17"/>
     </row>
-    <row r="67" spans="6:14" ht="39.75" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="67" spans="6:14" ht="39.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="F67" s="17"/>
       <c r="G67" s="17"/>
       <c r="H67" s="18"/>
@@ -2484,7 +2484,7 @@
       <c r="M67" s="19"/>
       <c r="N67" s="17"/>
     </row>
-    <row r="68" spans="6:14" ht="39.75" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="68" spans="6:14" ht="39.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="F68" s="17"/>
       <c r="G68" s="17"/>
       <c r="H68" s="18"/>
@@ -2495,7 +2495,7 @@
       <c r="M68" s="19"/>
       <c r="N68" s="17"/>
     </row>
-    <row r="69" spans="6:14" ht="39.75" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="69" spans="6:14" ht="39.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="F69" s="17"/>
       <c r="G69" s="17"/>
       <c r="H69" s="18"/>
@@ -2506,7 +2506,7 @@
       <c r="M69" s="19"/>
       <c r="N69" s="17"/>
     </row>
-    <row r="70" spans="6:14" ht="39.75" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="70" spans="6:14" ht="39.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="F70" s="17"/>
       <c r="G70" s="17"/>
       <c r="H70" s="18"/>
@@ -2517,7 +2517,7 @@
       <c r="M70" s="19"/>
       <c r="N70" s="17"/>
     </row>
-    <row r="71" spans="6:14" ht="39.75" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="71" spans="6:14" ht="39.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="F71" s="17"/>
       <c r="G71" s="17"/>
       <c r="H71" s="18"/>
@@ -2528,7 +2528,7 @@
       <c r="M71" s="19"/>
       <c r="N71" s="17"/>
     </row>
-    <row r="72" spans="6:14" ht="39.75" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="72" spans="6:14" ht="39.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="F72" s="17"/>
       <c r="G72" s="17"/>
       <c r="H72" s="18"/>
@@ -2539,7 +2539,7 @@
       <c r="M72" s="19"/>
       <c r="N72" s="17"/>
     </row>
-    <row r="73" spans="6:14" ht="39.75" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="73" spans="6:14" ht="39.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="F73" s="17"/>
       <c r="G73" s="17"/>
       <c r="H73" s="18"/>
@@ -2550,7 +2550,7 @@
       <c r="M73" s="19"/>
       <c r="N73" s="17"/>
     </row>
-    <row r="74" spans="6:14" ht="39.75" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="74" spans="6:14" ht="39.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="F74" s="17"/>
       <c r="G74" s="17"/>
       <c r="H74" s="18"/>
@@ -2561,7 +2561,7 @@
       <c r="M74" s="19"/>
       <c r="N74" s="17"/>
     </row>
-    <row r="75" spans="6:14" ht="39.75" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="75" spans="6:14" ht="39.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="F75" s="17"/>
       <c r="G75" s="17"/>
       <c r="H75" s="18"/>
@@ -2572,7 +2572,7 @@
       <c r="M75" s="19"/>
       <c r="N75" s="17"/>
     </row>
-    <row r="76" spans="6:14" ht="39.75" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="76" spans="6:14" ht="39.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="F76" s="17"/>
       <c r="G76" s="17"/>
       <c r="H76" s="18"/>
@@ -2583,7 +2583,7 @@
       <c r="M76" s="19"/>
       <c r="N76" s="17"/>
     </row>
-    <row r="77" spans="6:14" ht="39.75" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="77" spans="6:14" ht="39.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="F77" s="17"/>
       <c r="G77" s="17"/>
       <c r="H77" s="18"/>
@@ -2594,7 +2594,7 @@
       <c r="M77" s="19"/>
       <c r="N77" s="17"/>
     </row>
-    <row r="78" spans="6:14" ht="39.75" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="78" spans="6:14" ht="39.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="F78" s="17"/>
       <c r="G78" s="17"/>
       <c r="H78" s="18"/>
@@ -2605,7 +2605,7 @@
       <c r="M78" s="19"/>
       <c r="N78" s="17"/>
     </row>
-    <row r="79" spans="6:14" ht="39.75" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="79" spans="6:14" ht="39.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="F79" s="17"/>
       <c r="G79" s="17"/>
       <c r="H79" s="18"/>
@@ -2616,7 +2616,7 @@
       <c r="M79" s="19"/>
       <c r="N79" s="17"/>
     </row>
-    <row r="80" spans="6:14" ht="39.75" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="80" spans="6:14" ht="39.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="F80" s="17"/>
       <c r="G80" s="17"/>
       <c r="H80" s="18"/>
@@ -2627,7 +2627,7 @@
       <c r="M80" s="19"/>
       <c r="N80" s="17"/>
     </row>
-    <row r="81" spans="6:14" ht="39.75" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="81" spans="6:14" ht="39.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="F81" s="17"/>
       <c r="G81" s="17"/>
       <c r="H81" s="18"/>
@@ -2638,7 +2638,7 @@
       <c r="M81" s="19"/>
       <c r="N81" s="17"/>
     </row>
-    <row r="82" spans="6:14" ht="39.75" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="82" spans="6:14" ht="39.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="F82" s="17"/>
       <c r="G82" s="17"/>
       <c r="H82" s="18"/>
@@ -2649,7 +2649,7 @@
       <c r="M82" s="19"/>
       <c r="N82" s="17"/>
     </row>
-    <row r="83" spans="6:14" ht="39.75" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="83" spans="6:14" ht="39.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="F83" s="17"/>
       <c r="G83" s="17"/>
       <c r="H83" s="18"/>
@@ -2660,7 +2660,7 @@
       <c r="M83" s="19"/>
       <c r="N83" s="17"/>
     </row>
-    <row r="84" spans="6:14" ht="39.75" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="84" spans="6:14" ht="39.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="F84" s="17"/>
       <c r="G84" s="17"/>
       <c r="H84" s="18"/>
@@ -2671,7 +2671,7 @@
       <c r="M84" s="19"/>
       <c r="N84" s="17"/>
     </row>
-    <row r="85" spans="6:14" ht="39.75" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="85" spans="6:14" ht="39.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="F85" s="17"/>
       <c r="G85" s="17"/>
       <c r="H85" s="18"/>
@@ -2682,7 +2682,7 @@
       <c r="M85" s="19"/>
       <c r="N85" s="17"/>
     </row>
-    <row r="86" spans="6:14" ht="39.75" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="86" spans="6:14" ht="39.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="F86" s="17"/>
       <c r="G86" s="17"/>
       <c r="H86" s="18"/>
@@ -2693,7 +2693,7 @@
       <c r="M86" s="19"/>
       <c r="N86" s="17"/>
     </row>
-    <row r="87" spans="6:14" ht="39.75" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="87" spans="6:14" ht="39.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="F87" s="17"/>
       <c r="G87" s="17"/>
       <c r="H87" s="18"/>
@@ -2704,7 +2704,7 @@
       <c r="M87" s="19"/>
       <c r="N87" s="17"/>
     </row>
-    <row r="88" spans="6:14" ht="39.75" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="88" spans="6:14" ht="39.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="F88" s="17"/>
       <c r="G88" s="17"/>
       <c r="H88" s="18"/>
@@ -2715,7 +2715,7 @@
       <c r="M88" s="19"/>
       <c r="N88" s="17"/>
     </row>
-    <row r="89" spans="6:14" ht="39.75" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="89" spans="6:14" ht="39.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="F89" s="17"/>
       <c r="G89" s="17"/>
       <c r="H89" s="18"/>
@@ -2726,7 +2726,7 @@
       <c r="M89" s="19"/>
       <c r="N89" s="17"/>
     </row>
-    <row r="90" spans="6:14" ht="39.75" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="90" spans="6:14" ht="39.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="F90" s="17"/>
       <c r="G90" s="17"/>
       <c r="H90" s="18"/>
@@ -2737,7 +2737,7 @@
       <c r="M90" s="19"/>
       <c r="N90" s="17"/>
     </row>
-    <row r="91" spans="6:14" ht="39.75" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="91" spans="6:14" ht="39.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="F91" s="17"/>
       <c r="G91" s="17"/>
       <c r="H91" s="18"/>
@@ -2748,7 +2748,7 @@
       <c r="M91" s="19"/>
       <c r="N91" s="17"/>
     </row>
-    <row r="92" spans="6:14" ht="39.75" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="92" spans="6:14" ht="39.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="F92" s="17"/>
       <c r="G92" s="17"/>
       <c r="H92" s="18"/>
@@ -2759,7 +2759,7 @@
       <c r="M92" s="19"/>
       <c r="N92" s="17"/>
     </row>
-    <row r="93" spans="6:14" ht="39.75" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="93" spans="6:14" ht="39.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="F93" s="17"/>
       <c r="G93" s="17"/>
       <c r="H93" s="18"/>
@@ -2770,7 +2770,7 @@
       <c r="M93" s="19"/>
       <c r="N93" s="17"/>
     </row>
-    <row r="94" spans="6:14" ht="39.75" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="94" spans="6:14" ht="39.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="F94" s="17"/>
       <c r="G94" s="17"/>
       <c r="H94" s="18"/>
@@ -2781,7 +2781,7 @@
       <c r="M94" s="19"/>
       <c r="N94" s="17"/>
     </row>
-    <row r="95" spans="6:14" ht="39.75" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="95" spans="6:14" ht="39.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="F95" s="17"/>
       <c r="G95" s="17"/>
       <c r="H95" s="18"/>
@@ -2792,7 +2792,7 @@
       <c r="M95" s="19"/>
       <c r="N95" s="17"/>
     </row>
-    <row r="96" spans="6:14" ht="39.75" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="96" spans="6:14" ht="39.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="F96" s="17"/>
       <c r="G96" s="17"/>
       <c r="H96" s="18"/>
@@ -2803,7 +2803,7 @@
       <c r="M96" s="19"/>
       <c r="N96" s="17"/>
     </row>
-    <row r="97" spans="6:14" ht="39.75" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="97" spans="6:14" ht="39.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="F97" s="17"/>
       <c r="G97" s="17"/>
       <c r="H97" s="18"/>
@@ -2814,7 +2814,7 @@
       <c r="M97" s="19"/>
       <c r="N97" s="17"/>
     </row>
-    <row r="98" spans="6:14" ht="39.75" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="98" spans="6:14" ht="39.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="F98" s="17"/>
       <c r="G98" s="17"/>
       <c r="H98" s="18"/>
@@ -2825,7 +2825,7 @@
       <c r="M98" s="19"/>
       <c r="N98" s="17"/>
     </row>
-    <row r="99" spans="6:14" ht="39.75" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="99" spans="6:14" ht="39.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="F99" s="17"/>
       <c r="G99" s="17"/>
       <c r="H99" s="18"/>
@@ -2836,7 +2836,7 @@
       <c r="M99" s="19"/>
       <c r="N99" s="17"/>
     </row>
-    <row r="100" spans="6:14" ht="39.75" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="100" spans="6:14" ht="39.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="F100" s="17"/>
       <c r="G100" s="17"/>
       <c r="H100" s="18"/>
@@ -2847,7 +2847,7 @@
       <c r="M100" s="19"/>
       <c r="N100" s="17"/>
     </row>
-    <row r="101" spans="6:14" ht="39.75" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="101" spans="6:14" ht="39.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="F101" s="17"/>
       <c r="G101" s="17"/>
       <c r="H101" s="18"/>
@@ -2858,7 +2858,7 @@
       <c r="M101" s="19"/>
       <c r="N101" s="17"/>
     </row>
-    <row r="102" spans="6:14" ht="39.75" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="102" spans="6:14" ht="39.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="F102" s="17"/>
       <c r="G102" s="17"/>
       <c r="H102" s="18"/>
@@ -2869,7 +2869,7 @@
       <c r="M102" s="19"/>
       <c r="N102" s="17"/>
     </row>
-    <row r="103" spans="6:14" ht="39.75" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="103" spans="6:14" ht="39.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="F103" s="17"/>
       <c r="G103" s="17"/>
       <c r="H103" s="18"/>
@@ -2880,7 +2880,7 @@
       <c r="M103" s="19"/>
       <c r="N103" s="17"/>
     </row>
-    <row r="104" spans="6:14" ht="39.75" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="104" spans="6:14" ht="39.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="F104" s="17"/>
       <c r="G104" s="17"/>
       <c r="H104" s="18"/>
@@ -2891,7 +2891,7 @@
       <c r="M104" s="19"/>
       <c r="N104" s="17"/>
     </row>
-    <row r="105" spans="6:14" ht="39.75" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="105" spans="6:14" ht="39.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="F105" s="17"/>
       <c r="G105" s="17"/>
       <c r="H105" s="18"/>
@@ -2902,7 +2902,7 @@
       <c r="M105" s="19"/>
       <c r="N105" s="17"/>
     </row>
-    <row r="106" spans="6:14" ht="39.75" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="106" spans="6:14" ht="39.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="F106" s="17"/>
       <c r="G106" s="17"/>
       <c r="H106" s="18"/>
@@ -2913,7 +2913,7 @@
       <c r="M106" s="19"/>
       <c r="N106" s="17"/>
     </row>
-    <row r="107" spans="6:14" ht="39.75" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="107" spans="6:14" ht="39.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="F107" s="17"/>
       <c r="G107" s="17"/>
       <c r="H107" s="18"/>
@@ -2924,7 +2924,7 @@
       <c r="M107" s="19"/>
       <c r="N107" s="17"/>
     </row>
-    <row r="108" spans="6:14" ht="39.75" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="108" spans="6:14" ht="39.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="F108" s="17"/>
       <c r="G108" s="17"/>
       <c r="H108" s="18"/>
@@ -2935,7 +2935,7 @@
       <c r="M108" s="19"/>
       <c r="N108" s="17"/>
     </row>
-    <row r="109" spans="6:14" ht="39.75" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="109" spans="6:14" ht="39.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="F109" s="17"/>
       <c r="G109" s="17"/>
       <c r="H109" s="18"/>
@@ -2946,7 +2946,7 @@
       <c r="M109" s="19"/>
       <c r="N109" s="17"/>
     </row>
-    <row r="110" spans="6:14" ht="39.75" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="110" spans="6:14" ht="39.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="F110" s="17"/>
       <c r="G110" s="17"/>
       <c r="H110" s="18"/>
@@ -2957,7 +2957,7 @@
       <c r="M110" s="19"/>
       <c r="N110" s="17"/>
     </row>
-    <row r="111" spans="6:14" ht="39.75" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="111" spans="6:14" ht="39.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="F111" s="17"/>
       <c r="G111" s="17"/>
       <c r="H111" s="18"/>
@@ -2968,7 +2968,7 @@
       <c r="M111" s="19"/>
       <c r="N111" s="17"/>
     </row>
-    <row r="112" spans="6:14" ht="39.75" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="112" spans="6:14" ht="39.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="F112" s="17"/>
       <c r="G112" s="17"/>
       <c r="H112" s="18"/>
@@ -2979,7 +2979,7 @@
       <c r="M112" s="19"/>
       <c r="N112" s="17"/>
     </row>
-    <row r="113" spans="6:14" ht="39.75" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="113" spans="6:14" ht="39.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="F113" s="17"/>
       <c r="G113" s="17"/>
       <c r="H113" s="18"/>
@@ -2990,7 +2990,7 @@
       <c r="M113" s="19"/>
       <c r="N113" s="17"/>
     </row>
-    <row r="114" spans="6:14" ht="39.75" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="114" spans="6:14" ht="39.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="F114" s="17"/>
       <c r="G114" s="17"/>
       <c r="H114" s="18"/>
@@ -3001,7 +3001,7 @@
       <c r="M114" s="19"/>
       <c r="N114" s="17"/>
     </row>
-    <row r="115" spans="6:14" ht="39.75" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="115" spans="6:14" ht="39.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="F115" s="17"/>
       <c r="G115" s="17"/>
       <c r="H115" s="18"/>
@@ -3012,7 +3012,7 @@
       <c r="M115" s="19"/>
       <c r="N115" s="17"/>
     </row>
-    <row r="116" spans="6:14" ht="39.75" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="116" spans="6:14" ht="39.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="F116" s="17"/>
       <c r="G116" s="17"/>
       <c r="H116" s="18"/>
@@ -3023,7 +3023,7 @@
       <c r="M116" s="19"/>
       <c r="N116" s="17"/>
     </row>
-    <row r="117" spans="6:14" ht="39.75" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="117" spans="6:14" ht="39.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="F117" s="17"/>
       <c r="G117" s="17"/>
       <c r="H117" s="18"/>
@@ -3034,7 +3034,7 @@
       <c r="M117" s="19"/>
       <c r="N117" s="17"/>
     </row>
-    <row r="118" spans="6:14" ht="39.75" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="118" spans="6:14" ht="39.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="F118" s="17"/>
       <c r="G118" s="17"/>
       <c r="H118" s="18"/>
@@ -3045,7 +3045,7 @@
       <c r="M118" s="19"/>
       <c r="N118" s="17"/>
     </row>
-    <row r="119" spans="6:14" ht="39.75" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="119" spans="6:14" ht="39.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="F119" s="17"/>
       <c r="G119" s="17"/>
       <c r="H119" s="18"/>
@@ -3056,7 +3056,7 @@
       <c r="M119" s="19"/>
       <c r="N119" s="17"/>
     </row>
-    <row r="120" spans="6:14" ht="39.75" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="120" spans="6:14" ht="39.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="F120" s="17"/>
       <c r="G120" s="17"/>
       <c r="H120" s="18"/>
@@ -3067,7 +3067,7 @@
       <c r="M120" s="19"/>
       <c r="N120" s="17"/>
     </row>
-    <row r="121" spans="6:14" ht="39.75" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="121" spans="6:14" ht="39.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="F121" s="17"/>
       <c r="G121" s="17"/>
       <c r="H121" s="18"/>
@@ -3078,7 +3078,7 @@
       <c r="M121" s="19"/>
       <c r="N121" s="17"/>
     </row>
-    <row r="122" spans="6:14" ht="39.75" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="122" spans="6:14" ht="39.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="F122" s="17"/>
       <c r="G122" s="17"/>
       <c r="H122" s="18"/>
@@ -3089,7 +3089,7 @@
       <c r="M122" s="19"/>
       <c r="N122" s="17"/>
     </row>
-    <row r="123" spans="6:14" ht="39.75" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="123" spans="6:14" ht="39.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="F123" s="17"/>
       <c r="G123" s="17"/>
       <c r="H123" s="18"/>
@@ -3100,7 +3100,7 @@
       <c r="M123" s="19"/>
       <c r="N123" s="17"/>
     </row>
-    <row r="124" spans="6:14" ht="39.75" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="124" spans="6:14" ht="39.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="F124" s="17"/>
       <c r="G124" s="17"/>
       <c r="H124" s="18"/>
@@ -3111,7 +3111,7 @@
       <c r="M124" s="19"/>
       <c r="N124" s="17"/>
     </row>
-    <row r="125" spans="6:14" ht="39.75" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="125" spans="6:14" ht="39.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="F125" s="17"/>
       <c r="G125" s="17"/>
       <c r="H125" s="18"/>
@@ -3122,7 +3122,7 @@
       <c r="M125" s="19"/>
       <c r="N125" s="17"/>
     </row>
-    <row r="126" spans="6:14" ht="39.75" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="126" spans="6:14" ht="39.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="F126" s="17"/>
       <c r="G126" s="17"/>
       <c r="H126" s="18"/>
@@ -3133,7 +3133,7 @@
       <c r="M126" s="19"/>
       <c r="N126" s="17"/>
     </row>
-    <row r="127" spans="6:14" ht="39.75" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="127" spans="6:14" ht="39.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="F127" s="17"/>
       <c r="G127" s="17"/>
       <c r="H127" s="18"/>
@@ -3144,7 +3144,7 @@
       <c r="M127" s="19"/>
       <c r="N127" s="17"/>
     </row>
-    <row r="128" spans="6:14" ht="39.75" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="128" spans="6:14" ht="39.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="F128" s="17"/>
       <c r="G128" s="17"/>
       <c r="H128" s="18"/>
@@ -3155,7 +3155,7 @@
       <c r="M128" s="19"/>
       <c r="N128" s="17"/>
     </row>
-    <row r="129" spans="6:14" ht="39.75" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="129" spans="6:14" ht="39.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="F129" s="17"/>
       <c r="G129" s="17"/>
       <c r="H129" s="18"/>
@@ -3166,7 +3166,7 @@
       <c r="M129" s="19"/>
       <c r="N129" s="17"/>
     </row>
-    <row r="130" spans="6:14" ht="39.75" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="130" spans="6:14" ht="39.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="F130" s="17"/>
       <c r="G130" s="17"/>
       <c r="H130" s="18"/>
@@ -3177,7 +3177,7 @@
       <c r="M130" s="19"/>
       <c r="N130" s="17"/>
     </row>
-    <row r="131" spans="6:14" ht="39.75" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="131" spans="6:14" ht="39.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="F131" s="17"/>
       <c r="G131" s="17"/>
       <c r="H131" s="18"/>
@@ -3188,7 +3188,7 @@
       <c r="M131" s="19"/>
       <c r="N131" s="17"/>
     </row>
-    <row r="132" spans="6:14" ht="39.75" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="132" spans="6:14" ht="39.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="F132" s="17"/>
       <c r="G132" s="17"/>
       <c r="H132" s="18"/>
@@ -3199,7 +3199,7 @@
       <c r="M132" s="19"/>
       <c r="N132" s="17"/>
     </row>
-    <row r="133" spans="6:14" ht="39.75" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="133" spans="6:14" ht="39.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="F133" s="17"/>
       <c r="G133" s="17"/>
       <c r="H133" s="18"/>
@@ -3210,7 +3210,7 @@
       <c r="M133" s="19"/>
       <c r="N133" s="17"/>
     </row>
-    <row r="134" spans="6:14" ht="39.75" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="134" spans="6:14" ht="39.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="F134" s="17"/>
       <c r="G134" s="17"/>
       <c r="H134" s="18"/>
@@ -3221,7 +3221,7 @@
       <c r="M134" s="19"/>
       <c r="N134" s="17"/>
     </row>
-    <row r="135" spans="6:14" ht="39.75" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="135" spans="6:14" ht="39.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="F135" s="17"/>
       <c r="G135" s="17"/>
       <c r="H135" s="18"/>
@@ -3232,7 +3232,7 @@
       <c r="M135" s="19"/>
       <c r="N135" s="17"/>
     </row>
-    <row r="136" spans="6:14" ht="39.75" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="136" spans="6:14" ht="39.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="F136" s="17"/>
       <c r="G136" s="17"/>
       <c r="H136" s="18"/>
@@ -3243,7 +3243,7 @@
       <c r="M136" s="19"/>
       <c r="N136" s="17"/>
     </row>
-    <row r="137" spans="6:14" ht="39.75" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="137" spans="6:14" ht="39.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="F137" s="17"/>
       <c r="G137" s="17"/>
       <c r="H137" s="18"/>
@@ -3254,7 +3254,7 @@
       <c r="M137" s="19"/>
       <c r="N137" s="17"/>
     </row>
-    <row r="138" spans="6:14" ht="39.75" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="138" spans="6:14" ht="39.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="F138" s="17"/>
       <c r="G138" s="17"/>
       <c r="H138" s="18"/>
@@ -3265,7 +3265,7 @@
       <c r="M138" s="19"/>
       <c r="N138" s="17"/>
     </row>
-    <row r="139" spans="6:14" ht="39.75" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="139" spans="6:14" ht="39.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="F139" s="17"/>
       <c r="G139" s="17"/>
       <c r="H139" s="18"/>
@@ -3276,7 +3276,7 @@
       <c r="M139" s="19"/>
       <c r="N139" s="17"/>
     </row>
-    <row r="140" spans="6:14" ht="39.75" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="140" spans="6:14" ht="39.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="F140" s="17"/>
       <c r="G140" s="17"/>
       <c r="H140" s="18"/>
@@ -3287,7 +3287,7 @@
       <c r="M140" s="19"/>
       <c r="N140" s="17"/>
     </row>
-    <row r="141" spans="6:14" ht="39.75" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="141" spans="6:14" ht="39.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="F141" s="17"/>
       <c r="G141" s="17"/>
       <c r="H141" s="18"/>
@@ -3298,7 +3298,7 @@
       <c r="M141" s="19"/>
       <c r="N141" s="17"/>
     </row>
-    <row r="142" spans="6:14" ht="39.75" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="142" spans="6:14" ht="39.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="F142" s="17"/>
       <c r="G142" s="17"/>
       <c r="H142" s="18"/>
@@ -3309,7 +3309,7 @@
       <c r="M142" s="19"/>
       <c r="N142" s="17"/>
     </row>
-    <row r="143" spans="6:14" ht="39.75" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="143" spans="6:14" ht="39.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="F143" s="17"/>
       <c r="G143" s="17"/>
       <c r="H143" s="18"/>
@@ -3320,7 +3320,7 @@
       <c r="M143" s="19"/>
       <c r="N143" s="17"/>
     </row>
-    <row r="144" spans="6:14" ht="39.75" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="144" spans="6:14" ht="39.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="F144" s="17"/>
       <c r="G144" s="17"/>
       <c r="H144" s="18"/>
@@ -3331,7 +3331,7 @@
       <c r="M144" s="19"/>
       <c r="N144" s="17"/>
     </row>
-    <row r="145" spans="6:14" ht="39.75" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="145" spans="6:14" ht="39.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="F145" s="17"/>
       <c r="G145" s="17"/>
       <c r="H145" s="18"/>
@@ -3342,7 +3342,7 @@
       <c r="M145" s="19"/>
       <c r="N145" s="17"/>
     </row>
-    <row r="146" spans="6:14" ht="39.75" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="146" spans="6:14" ht="39.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="F146" s="17"/>
       <c r="G146" s="17"/>
       <c r="H146" s="18"/>
@@ -3353,7 +3353,7 @@
       <c r="M146" s="19"/>
       <c r="N146" s="17"/>
     </row>
-    <row r="147" spans="6:14" ht="39.75" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="147" spans="6:14" ht="39.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="F147" s="17"/>
       <c r="G147" s="17"/>
       <c r="H147" s="18"/>
@@ -3364,7 +3364,7 @@
       <c r="M147" s="19"/>
       <c r="N147" s="17"/>
     </row>
-    <row r="148" spans="6:14" ht="39.75" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="148" spans="6:14" ht="39.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="F148" s="17"/>
       <c r="G148" s="17"/>
       <c r="H148" s="18"/>
@@ -3375,9 +3375,9 @@
       <c r="M148" s="19"/>
       <c r="N148" s="17"/>
     </row>
-    <row r="149" spans="6:14" ht="39.75" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="149" spans="6:14" ht="39.75" customHeight="1" x14ac:dyDescent="0.4"/>
   </sheetData>
-  <autoFilter ref="F4:N4"/>
+  <autoFilter ref="F4:N39"/>
   <mergeCells count="1">
     <mergeCell ref="F2:N2"/>
   </mergeCells>
@@ -3435,631 +3435,630 @@
       <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultColWidth="8.69921875" defaultRowHeight="16.8" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="1" width="50.58203125" style="1" customWidth="1"/>
+    <col min="1" max="1" width="50.59765625" style="1" customWidth="1"/>
     <col min="2" max="2" width="53" style="1" customWidth="1"/>
     <col min="3" max="3" width="100" style="1" customWidth="1"/>
-    <col min="4" max="4" width="27.25" style="3" customWidth="1"/>
-    <col min="5" max="16384" width="8.6640625" style="1"/>
+    <col min="4" max="4" width="27.19921875" style="3" customWidth="1"/>
+    <col min="5" max="16384" width="8.69921875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="56" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A1" s="33" t="s">
+    <row r="1" spans="1:9" ht="55.95" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A1" s="38" t="s">
         <v>85</v>
       </c>
-      <c r="B1" s="34"/>
-      <c r="C1" s="34"/>
-      <c r="D1" s="35"/>
+      <c r="B1" s="39"/>
+      <c r="C1" s="39"/>
+      <c r="D1" s="40"/>
       <c r="E1" s="20"/>
     </row>
-    <row r="2" spans="1:9" s="5" customFormat="1" ht="18.5" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:9" s="5" customFormat="1" ht="18.45" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A2" s="21"/>
       <c r="B2" s="22"/>
       <c r="C2" s="22"/>
       <c r="D2" s="23"/>
       <c r="E2" s="24"/>
     </row>
-    <row r="3" spans="1:9" ht="39.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="3" spans="1:9" ht="39.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A3" s="27" t="s">
         <v>0</v>
       </c>
-      <c r="B3" s="36" t="s">
+      <c r="B3" s="41" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="36"/>
-      <c r="D3" s="39" t="s">
+      <c r="C3" s="41"/>
+      <c r="D3" s="29" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:9" ht="39.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="4" spans="1:9" ht="39.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A4" s="10" t="s">
         <v>68</v>
       </c>
-      <c r="B4" s="37" t="s">
+      <c r="B4" s="42" t="s">
         <v>69</v>
       </c>
-      <c r="C4" s="38"/>
-      <c r="D4" s="40" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" s="25" customFormat="1" ht="39.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="C4" s="43"/>
+      <c r="D4" s="30" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" s="25" customFormat="1" ht="39.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A5" s="10" t="s">
         <v>40</v>
       </c>
-      <c r="B5" s="37" t="s">
+      <c r="B5" s="42" t="s">
         <v>41</v>
       </c>
-      <c r="C5" s="38"/>
-      <c r="D5" s="41" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" ht="39.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="C5" s="43"/>
+      <c r="D5" s="31" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" ht="39.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A6" s="10" t="s">
         <v>42</v>
       </c>
-      <c r="B6" s="31" t="s">
+      <c r="B6" s="36" t="s">
         <v>43</v>
       </c>
-      <c r="C6" s="32"/>
-      <c r="D6" s="41" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" ht="39.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="C6" s="37"/>
+      <c r="D6" s="31" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" ht="39.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A7" s="10" t="s">
         <v>44</v>
       </c>
-      <c r="B7" s="31" t="s">
+      <c r="B7" s="36" t="s">
         <v>45</v>
       </c>
-      <c r="C7" s="32"/>
-      <c r="D7" s="41" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" ht="39.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="C7" s="37"/>
+      <c r="D7" s="31" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" ht="39.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A8" s="10" t="s">
         <v>46</v>
       </c>
-      <c r="B8" s="31" t="s">
+      <c r="B8" s="36" t="s">
         <v>47</v>
       </c>
-      <c r="C8" s="32"/>
-      <c r="D8" s="41" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9" ht="39.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="C8" s="37"/>
+      <c r="D8" s="31" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" ht="39.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A9" s="10" t="s">
         <v>48</v>
       </c>
-      <c r="B9" s="31" t="s">
+      <c r="B9" s="36" t="s">
         <v>49</v>
       </c>
-      <c r="C9" s="32"/>
-      <c r="D9" s="41" t="s">
+      <c r="C9" s="37"/>
+      <c r="D9" s="31" t="s">
         <v>5</v>
       </c>
       <c r="I9" s="26"/>
     </row>
-    <row r="10" spans="1:9" ht="39.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="10" spans="1:9" ht="39.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A10" s="10" t="s">
         <v>83</v>
       </c>
-      <c r="B10" s="31" t="s">
+      <c r="B10" s="36" t="s">
         <v>50</v>
       </c>
-      <c r="C10" s="32"/>
-      <c r="D10" s="41" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9" ht="39.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="C10" s="37"/>
+      <c r="D10" s="31" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" ht="39.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A11" s="10" t="s">
         <v>51</v>
       </c>
-      <c r="B11" s="31" t="s">
+      <c r="B11" s="36" t="s">
         <v>52</v>
       </c>
-      <c r="C11" s="32"/>
-      <c r="D11" s="41" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9" ht="39.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="C11" s="37"/>
+      <c r="D11" s="31" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" ht="39.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A12" s="10" t="s">
         <v>53</v>
       </c>
-      <c r="B12" s="31" t="s">
+      <c r="B12" s="36" t="s">
         <v>54</v>
       </c>
-      <c r="C12" s="32"/>
-      <c r="D12" s="41" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="13" spans="1:9" ht="39.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="C12" s="37"/>
+      <c r="D12" s="31" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" ht="39.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A13" s="10" t="s">
         <v>70</v>
       </c>
-      <c r="B13" s="31" t="s">
+      <c r="B13" s="36" t="s">
         <v>55</v>
       </c>
-      <c r="C13" s="32"/>
-      <c r="D13" s="41" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="14" spans="1:9" ht="39.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="C13" s="37"/>
+      <c r="D13" s="31" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" ht="39.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A14" s="10" t="s">
         <v>56</v>
       </c>
-      <c r="B14" s="31" t="s">
+      <c r="B14" s="36" t="s">
         <v>57</v>
       </c>
-      <c r="C14" s="32"/>
-      <c r="D14" s="41" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="15" spans="1:9" ht="39.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="C14" s="37"/>
+      <c r="D14" s="31" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" ht="39.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A15" s="10" t="s">
         <v>58</v>
       </c>
-      <c r="B15" s="31" t="s">
+      <c r="B15" s="36" t="s">
         <v>59</v>
       </c>
-      <c r="C15" s="32"/>
-      <c r="D15" s="41" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="16" spans="1:9" ht="39.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="C15" s="37"/>
+      <c r="D15" s="31" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" ht="39.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A16" s="10" t="s">
         <v>60</v>
       </c>
-      <c r="B16" s="31" t="s">
+      <c r="B16" s="36" t="s">
         <v>61</v>
       </c>
-      <c r="C16" s="32"/>
-      <c r="D16" s="41" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" ht="39.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="C16" s="37"/>
+      <c r="D16" s="31" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" ht="39.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A17" s="10" t="s">
         <v>62</v>
       </c>
-      <c r="B17" s="31" t="s">
+      <c r="B17" s="36" t="s">
         <v>63</v>
       </c>
-      <c r="C17" s="32"/>
-      <c r="D17" s="41" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" ht="39.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="C17" s="37"/>
+      <c r="D17" s="31" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" ht="39.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A18" s="10" t="s">
         <v>64</v>
       </c>
-      <c r="B18" s="31" t="s">
+      <c r="B18" s="36" t="s">
         <v>65</v>
       </c>
-      <c r="C18" s="32"/>
-      <c r="D18" s="41" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" ht="39.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="C18" s="37"/>
+      <c r="D18" s="31" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" ht="39.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A19" s="10"/>
-      <c r="B19" s="31"/>
-      <c r="C19" s="32"/>
-      <c r="D19" s="42"/>
-    </row>
-    <row r="20" spans="1:4" ht="39.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="B19" s="36"/>
+      <c r="C19" s="37"/>
+      <c r="D19" s="32"/>
+    </row>
+    <row r="20" spans="1:4" ht="39.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A20" s="10"/>
-      <c r="B20" s="31"/>
-      <c r="C20" s="32"/>
-      <c r="D20" s="42"/>
-    </row>
-    <row r="21" spans="1:4" ht="39.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="B20" s="36"/>
+      <c r="C20" s="37"/>
+      <c r="D20" s="32"/>
+    </row>
+    <row r="21" spans="1:4" ht="39.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A21" s="10"/>
-      <c r="B21" s="31"/>
-      <c r="C21" s="32"/>
-      <c r="D21" s="42"/>
-    </row>
-    <row r="22" spans="1:4" ht="39.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="B21" s="36"/>
+      <c r="C21" s="37"/>
+      <c r="D21" s="32"/>
+    </row>
+    <row r="22" spans="1:4" ht="39.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A22" s="10"/>
-      <c r="B22" s="31"/>
-      <c r="C22" s="32"/>
-      <c r="D22" s="42"/>
-    </row>
-    <row r="23" spans="1:4" ht="39.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="B22" s="36"/>
+      <c r="C22" s="37"/>
+      <c r="D22" s="32"/>
+    </row>
+    <row r="23" spans="1:4" ht="39.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A23" s="10"/>
-      <c r="B23" s="31"/>
-      <c r="C23" s="32"/>
-      <c r="D23" s="42"/>
-    </row>
-    <row r="24" spans="1:4" ht="39.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="B23" s="36"/>
+      <c r="C23" s="37"/>
+      <c r="D23" s="32"/>
+    </row>
+    <row r="24" spans="1:4" ht="39.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A24" s="10"/>
-      <c r="B24" s="31"/>
-      <c r="C24" s="32"/>
-      <c r="D24" s="43"/>
-    </row>
-    <row r="25" spans="1:4" ht="39.75" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="B24" s="36"/>
+      <c r="C24" s="37"/>
+      <c r="D24" s="33"/>
+    </row>
+    <row r="25" spans="1:4" ht="39.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A25" s="17"/>
       <c r="B25" s="28"/>
       <c r="C25" s="28"/>
       <c r="D25" s="19"/>
     </row>
-    <row r="26" spans="1:4" ht="39.75" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="26" spans="1:4" ht="39.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A26" s="17"/>
       <c r="B26" s="28"/>
       <c r="C26" s="28"/>
       <c r="D26" s="19"/>
     </row>
-    <row r="27" spans="1:4" ht="39.75" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="27" spans="1:4" ht="39.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A27" s="17"/>
       <c r="B27" s="28"/>
       <c r="C27" s="28"/>
       <c r="D27" s="19"/>
     </row>
-    <row r="28" spans="1:4" ht="39.75" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="28" spans="1:4" ht="39.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A28" s="17"/>
       <c r="B28" s="28"/>
       <c r="C28" s="28"/>
       <c r="D28" s="19"/>
     </row>
-    <row r="29" spans="1:4" ht="39.75" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="29" spans="1:4" ht="39.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A29" s="17"/>
       <c r="B29" s="28"/>
       <c r="C29" s="28"/>
       <c r="D29" s="19"/>
     </row>
-    <row r="30" spans="1:4" ht="39.75" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="30" spans="1:4" ht="39.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A30" s="17"/>
       <c r="B30" s="28"/>
       <c r="C30" s="28"/>
       <c r="D30" s="19"/>
     </row>
-    <row r="31" spans="1:4" ht="39.75" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="31" spans="1:4" ht="39.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A31" s="17"/>
       <c r="B31" s="28"/>
       <c r="C31" s="28"/>
       <c r="D31" s="19"/>
     </row>
-    <row r="32" spans="1:4" ht="39.75" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="32" spans="1:4" ht="39.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A32" s="17"/>
       <c r="B32" s="28"/>
       <c r="C32" s="28"/>
       <c r="D32" s="19"/>
     </row>
-    <row r="33" spans="1:4" ht="39.75" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="33" spans="1:4" ht="39.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A33" s="17"/>
       <c r="B33" s="28"/>
       <c r="C33" s="28"/>
       <c r="D33" s="19"/>
     </row>
-    <row r="34" spans="1:4" ht="39.75" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="34" spans="1:4" ht="39.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A34" s="17"/>
       <c r="B34" s="28"/>
       <c r="C34" s="28"/>
       <c r="D34" s="19"/>
     </row>
-    <row r="35" spans="1:4" ht="39.75" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="35" spans="1:4" ht="39.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A35" s="17"/>
       <c r="B35" s="28"/>
       <c r="C35" s="28"/>
       <c r="D35" s="19"/>
     </row>
-    <row r="36" spans="1:4" ht="39.75" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="36" spans="1:4" ht="39.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A36" s="17"/>
       <c r="B36" s="28"/>
       <c r="C36" s="28"/>
       <c r="D36" s="19"/>
     </row>
-    <row r="37" spans="1:4" ht="39.75" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="37" spans="1:4" ht="39.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A37" s="17"/>
       <c r="B37" s="28"/>
       <c r="C37" s="28"/>
       <c r="D37" s="19"/>
     </row>
-    <row r="38" spans="1:4" ht="39.75" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="38" spans="1:4" ht="39.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A38" s="17"/>
       <c r="B38" s="28"/>
       <c r="C38" s="28"/>
       <c r="D38" s="19"/>
     </row>
-    <row r="39" spans="1:4" ht="39.75" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="39" spans="1:4" ht="39.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A39" s="17"/>
       <c r="B39" s="28"/>
       <c r="C39" s="28"/>
       <c r="D39" s="19"/>
     </row>
-    <row r="40" spans="1:4" ht="39.75" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="40" spans="1:4" ht="39.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A40" s="17"/>
       <c r="B40" s="28"/>
       <c r="C40" s="28"/>
       <c r="D40" s="19"/>
     </row>
-    <row r="41" spans="1:4" ht="39.75" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="41" spans="1:4" ht="39.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B41" s="20"/>
       <c r="C41" s="20"/>
     </row>
-    <row r="42" spans="1:4" ht="39.75" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="42" spans="1:4" ht="39.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B42" s="20"/>
       <c r="C42" s="20"/>
     </row>
-    <row r="43" spans="1:4" ht="39.75" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="43" spans="1:4" ht="39.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B43" s="20"/>
       <c r="C43" s="20"/>
     </row>
-    <row r="44" spans="1:4" ht="39.75" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="44" spans="1:4" ht="39.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B44" s="20"/>
       <c r="C44" s="20"/>
     </row>
-    <row r="45" spans="1:4" ht="39.75" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="45" spans="1:4" ht="39.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B45" s="20"/>
       <c r="C45" s="20"/>
     </row>
-    <row r="46" spans="1:4" ht="39.75" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="46" spans="1:4" ht="39.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B46" s="20"/>
       <c r="C46" s="20"/>
     </row>
-    <row r="47" spans="1:4" ht="39.75" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="47" spans="1:4" ht="39.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B47" s="20"/>
       <c r="C47" s="20"/>
     </row>
-    <row r="48" spans="1:4" ht="39.75" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="48" spans="1:4" ht="39.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B48" s="20"/>
       <c r="C48" s="20"/>
     </row>
-    <row r="49" spans="2:3" ht="39.75" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="49" spans="2:3" ht="39.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B49" s="20"/>
       <c r="C49" s="20"/>
     </row>
-    <row r="50" spans="2:3" ht="39.75" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="50" spans="2:3" ht="39.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B50" s="20"/>
       <c r="C50" s="20"/>
     </row>
-    <row r="51" spans="2:3" ht="39.75" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="51" spans="2:3" ht="39.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B51" s="20"/>
       <c r="C51" s="20"/>
     </row>
-    <row r="52" spans="2:3" ht="39.75" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="52" spans="2:3" ht="39.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B52" s="20"/>
       <c r="C52" s="20"/>
     </row>
-    <row r="53" spans="2:3" ht="39.75" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="53" spans="2:3" ht="39.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B53" s="20"/>
       <c r="C53" s="20"/>
     </row>
-    <row r="54" spans="2:3" ht="39.75" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="54" spans="2:3" ht="39.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B54" s="20"/>
       <c r="C54" s="20"/>
     </row>
-    <row r="55" spans="2:3" ht="39.75" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="55" spans="2:3" ht="39.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B55" s="20"/>
       <c r="C55" s="20"/>
     </row>
-    <row r="56" spans="2:3" ht="39.75" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="56" spans="2:3" ht="39.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B56" s="20"/>
       <c r="C56" s="20"/>
     </row>
-    <row r="57" spans="2:3" ht="39.75" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="57" spans="2:3" ht="39.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B57" s="20"/>
       <c r="C57" s="20"/>
     </row>
-    <row r="58" spans="2:3" ht="39.75" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="58" spans="2:3" ht="39.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B58" s="20"/>
       <c r="C58" s="20"/>
     </row>
-    <row r="59" spans="2:3" ht="39.75" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="59" spans="2:3" ht="39.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B59" s="20"/>
       <c r="C59" s="20"/>
     </row>
-    <row r="60" spans="2:3" ht="39.75" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="60" spans="2:3" ht="39.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B60" s="20"/>
       <c r="C60" s="20"/>
     </row>
-    <row r="61" spans="2:3" ht="39.75" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="61" spans="2:3" ht="39.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B61" s="20"/>
       <c r="C61" s="20"/>
     </row>
-    <row r="62" spans="2:3" ht="39.75" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="62" spans="2:3" ht="39.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B62" s="20"/>
       <c r="C62" s="20"/>
     </row>
-    <row r="63" spans="2:3" ht="39.75" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="64" spans="2:3" ht="39.75" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="65" ht="39.75" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="66" ht="39.75" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="67" ht="39.75" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="68" ht="39.75" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="69" ht="39.75" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="70" ht="39.75" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="71" ht="39.75" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="72" ht="39.75" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="73" ht="39.75" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="74" ht="39.75" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="75" ht="39.75" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="76" ht="39.75" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="77" ht="39.75" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="78" ht="39.75" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="79" ht="39.75" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="80" ht="39.75" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="81" ht="39.75" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="82" ht="39.75" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="83" ht="39.75" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="84" ht="39.75" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="85" ht="39.75" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="86" ht="39.75" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="87" ht="39.75" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="88" ht="39.75" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="89" ht="39.75" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="90" ht="39.75" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="91" ht="39.75" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="92" ht="39.75" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="93" ht="39.75" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="94" ht="39.75" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="95" ht="39.75" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="96" ht="39.75" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="97" ht="39.75" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="98" ht="39.75" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="99" ht="39.75" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="100" ht="39.75" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="101" ht="39.75" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="102" ht="39.75" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="103" ht="39.75" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="104" ht="39.75" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="105" ht="39.75" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="106" ht="39.75" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="107" ht="39.75" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="108" ht="39.75" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="109" ht="39.75" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="110" ht="39.75" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="111" ht="39.75" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="112" ht="39.75" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="113" ht="39.75" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="114" ht="39.75" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="115" ht="39.75" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="116" ht="39.75" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="117" ht="39.75" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="118" ht="39.75" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="119" ht="39.75" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="120" ht="39.75" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="121" ht="39.75" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="122" ht="39.75" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="123" ht="39.75" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="124" ht="39.75" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="125" ht="39.75" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="126" ht="39.75" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="127" ht="39.75" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="128" ht="39.75" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="129" ht="39.75" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="130" ht="39.75" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="131" ht="39.75" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="132" ht="39.75" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="133" ht="39.75" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="134" ht="39.75" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="135" ht="39.75" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="136" ht="39.75" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="137" ht="39.75" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="138" ht="39.75" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="139" ht="39.75" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="140" ht="39.75" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="141" ht="39.75" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="142" ht="39.75" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="143" ht="39.75" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="144" ht="39.75" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="145" ht="39.75" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="146" ht="39.75" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="147" ht="39.75" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="148" ht="39.75" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="149" ht="39.75" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="150" ht="39.75" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="151" ht="39.75" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="152" ht="39.75" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="153" ht="39.75" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="154" ht="39.75" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="155" ht="39.75" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="156" ht="39.75" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="157" ht="39.75" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="158" ht="39.75" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="159" ht="39.75" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="160" ht="39.75" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="161" ht="39.75" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="162" ht="39.75" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="163" ht="39.75" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="164" ht="39.75" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="165" ht="39.75" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="166" ht="39.75" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="167" ht="39.75" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="168" ht="39.75" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="169" ht="39.75" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="170" ht="39.75" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="171" ht="39.75" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="172" ht="39.75" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="173" ht="39.75" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="174" ht="39.75" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="175" ht="39.75" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="176" ht="39.75" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="177" ht="39.75" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="178" ht="39.75" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="179" ht="39.75" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="180" ht="39.75" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="181" ht="39.75" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="182" ht="39.75" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="183" ht="39.75" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="184" ht="39.75" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="185" ht="39.75" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="186" ht="39.75" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="187" ht="39.75" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="188" ht="39.75" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="189" ht="39.75" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="190" ht="39.75" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="191" ht="39.75" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="192" ht="39.75" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="193" ht="39.75" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="194" ht="39.75" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="195" ht="39.75" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="196" ht="39.75" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="197" ht="39.75" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="198" ht="39.75" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="199" ht="39.75" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="200" ht="39.75" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="201" ht="39.75" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="202" ht="39.75" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="203" ht="39.75" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="204" ht="39.75" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="205" ht="39.75" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="206" ht="39.75" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="207" ht="39.75" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="208" ht="39.75" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="209" ht="39.75" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="210" ht="39.75" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="211" ht="39.75" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="212" ht="39.75" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="213" ht="39.75" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="214" ht="39.75" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="215" ht="39.75" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="216" ht="39.75" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="217" ht="39.75" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="218" ht="39.75" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="219" ht="39.75" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="220" ht="39.75" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="221" ht="39.75" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="222" ht="39.75" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="223" ht="39.75" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="224" ht="39.75" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="225" ht="39.75" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="226" ht="39.75" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="227" ht="39.75" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="228" ht="39.75" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="229" ht="39.75" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="230" ht="39.75" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="231" ht="39.75" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="232" ht="39.75" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="233" ht="39.75" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="234" ht="39.75" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="235" ht="39.75" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="236" ht="39.75" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="237" ht="39.75" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="238" ht="39.75" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="239" ht="39.75" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="240" ht="39.75" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="241" ht="39.75" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="63" spans="2:3" ht="39.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="64" spans="2:3" ht="39.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="65" ht="39.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="66" ht="39.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="67" ht="39.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="68" ht="39.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="69" ht="39.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="70" ht="39.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="71" ht="39.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="72" ht="39.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="73" ht="39.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="74" ht="39.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="75" ht="39.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="76" ht="39.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="77" ht="39.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="78" ht="39.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="79" ht="39.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="80" ht="39.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="81" ht="39.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="82" ht="39.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="83" ht="39.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="84" ht="39.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="85" ht="39.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="86" ht="39.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="87" ht="39.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="88" ht="39.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="89" ht="39.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="90" ht="39.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="91" ht="39.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="92" ht="39.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="93" ht="39.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="94" ht="39.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="95" ht="39.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="96" ht="39.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="97" ht="39.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="98" ht="39.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="99" ht="39.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="100" ht="39.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="101" ht="39.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="102" ht="39.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="103" ht="39.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="104" ht="39.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="105" ht="39.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="106" ht="39.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="107" ht="39.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="108" ht="39.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="109" ht="39.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="110" ht="39.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="111" ht="39.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="112" ht="39.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="113" ht="39.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="114" ht="39.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="115" ht="39.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="116" ht="39.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="117" ht="39.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="118" ht="39.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="119" ht="39.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="120" ht="39.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="121" ht="39.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="122" ht="39.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="123" ht="39.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="124" ht="39.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="125" ht="39.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="126" ht="39.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="127" ht="39.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="128" ht="39.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="129" ht="39.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="130" ht="39.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="131" ht="39.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="132" ht="39.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="133" ht="39.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="134" ht="39.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="135" ht="39.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="136" ht="39.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="137" ht="39.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="138" ht="39.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="139" ht="39.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="140" ht="39.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="141" ht="39.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="142" ht="39.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="143" ht="39.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="144" ht="39.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="145" ht="39.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="146" ht="39.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="147" ht="39.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="148" ht="39.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="149" ht="39.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="150" ht="39.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="151" ht="39.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="152" ht="39.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="153" ht="39.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="154" ht="39.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="155" ht="39.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="156" ht="39.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="157" ht="39.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="158" ht="39.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="159" ht="39.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="160" ht="39.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="161" ht="39.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="162" ht="39.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="163" ht="39.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="164" ht="39.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="165" ht="39.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="166" ht="39.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="167" ht="39.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="168" ht="39.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="169" ht="39.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="170" ht="39.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="171" ht="39.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="172" ht="39.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="173" ht="39.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="174" ht="39.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="175" ht="39.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="176" ht="39.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="177" ht="39.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="178" ht="39.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="179" ht="39.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="180" ht="39.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="181" ht="39.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="182" ht="39.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="183" ht="39.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="184" ht="39.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="185" ht="39.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="186" ht="39.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="187" ht="39.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="188" ht="39.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="189" ht="39.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="190" ht="39.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="191" ht="39.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="192" ht="39.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="193" ht="39.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="194" ht="39.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="195" ht="39.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="196" ht="39.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="197" ht="39.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="198" ht="39.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="199" ht="39.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="200" ht="39.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="201" ht="39.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="202" ht="39.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="203" ht="39.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="204" ht="39.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="205" ht="39.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="206" ht="39.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="207" ht="39.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="208" ht="39.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="209" ht="39.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="210" ht="39.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="211" ht="39.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="212" ht="39.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="213" ht="39.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="214" ht="39.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="215" ht="39.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="216" ht="39.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="217" ht="39.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="218" ht="39.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="219" ht="39.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="220" ht="39.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="221" ht="39.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="222" ht="39.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="223" ht="39.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="224" ht="39.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="225" ht="39.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="226" ht="39.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="227" ht="39.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="228" ht="39.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="229" ht="39.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="230" ht="39.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="231" ht="39.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="232" ht="39.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="233" ht="39.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="234" ht="39.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="235" ht="39.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="236" ht="39.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="237" ht="39.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="238" ht="39.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="239" ht="39.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="240" ht="39.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="241" ht="39.75" customHeight="1" x14ac:dyDescent="0.4"/>
   </sheetData>
   <mergeCells count="23">
-    <mergeCell ref="B7:C7"/>
-    <mergeCell ref="A1:D1"/>
-    <mergeCell ref="B3:C3"/>
-    <mergeCell ref="B4:C4"/>
-    <mergeCell ref="B5:C5"/>
-    <mergeCell ref="B6:C6"/>
+    <mergeCell ref="B20:C20"/>
+    <mergeCell ref="B21:C21"/>
+    <mergeCell ref="B22:C22"/>
+    <mergeCell ref="B23:C23"/>
+    <mergeCell ref="B24:C24"/>
     <mergeCell ref="B19:C19"/>
     <mergeCell ref="B8:C8"/>
     <mergeCell ref="B9:C9"/>
@@ -4072,11 +4071,12 @@
     <mergeCell ref="B16:C16"/>
     <mergeCell ref="B17:C17"/>
     <mergeCell ref="B18:C18"/>
-    <mergeCell ref="B20:C20"/>
-    <mergeCell ref="B21:C21"/>
-    <mergeCell ref="B22:C22"/>
-    <mergeCell ref="B23:C23"/>
-    <mergeCell ref="B24:C24"/>
+    <mergeCell ref="B7:C7"/>
+    <mergeCell ref="A1:D1"/>
+    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="B4:C4"/>
+    <mergeCell ref="B5:C5"/>
+    <mergeCell ref="B6:C6"/>
   </mergeCells>
   <conditionalFormatting sqref="C2">
     <cfRule type="containsText" dxfId="2" priority="1" operator="containsText" text="Desejável">

</xml_diff>